<commit_message>
refactor: organize code into app/ package (gui/services/reports), add backward-compat shims, keep main.py in root; tests green
</commit_message>
<xml_diff>
--- a/excel_menu_gui/templates/Шаблон меню пример.xlsx
+++ b/excel_menu_gui/templates/Шаблон меню пример.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katya\Desktop\menurepit\excel_menu_gui\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ADE195-0B05-4635-96AA-5A3BE78AE485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5DCD69-2003-490B-886C-3057B8DE5114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="447" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="447" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Касса" sheetId="1" r:id="rId1"/>
@@ -1542,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C42"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1553,15 +1553,14 @@
     <col min="1" max="1" width="41.7265625" customWidth="1"/>
     <col min="2" max="2" width="12.54296875" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="47.7265625" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
-    <col min="8" max="9" width="6.54296875" customWidth="1"/>
-    <col min="10" max="10" width="5.453125" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="8" width="6.54296875" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1569,51 +1568,47 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="79" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="78"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="77" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="78"/>
       <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="80" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="78"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="77" t="s">
+      <c r="D3" s="77" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="78"/>
       <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="81" t="s">
         <v>4</v>
       </c>
@@ -1622,14 +1617,13 @@
       <c r="D5" s="78"/>
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="18"/>
-    </row>
-    <row r="6" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="20"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1639,609 +1633,571 @@
       <c r="C6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="E6" s="22" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="21"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="73"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="18"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="66"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="60"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="66"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-    </row>
-    <row r="12" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="73"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="66"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="60"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="73"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="66"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="60"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="66"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="60"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="68"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="69"/>
       <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="60"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="60"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="60"/>
       <c r="M16" s="60"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="18"/>
-      <c r="P17" s="60"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="18"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="18"/>
+      <c r="O17" s="60"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>11</v>
       </c>
+      <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="18"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="74"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="71"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="18"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="74"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="18"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="73"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="18"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="18"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="18"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="18"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="3"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="18"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="74"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="6"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="74"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="10"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="18"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="70"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="6"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="70"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="60"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="60"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="3"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="6"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="3"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="6"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="3"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="6"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="3"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="18"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="6"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="3"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="18"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="6"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="3"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="18"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="6"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="3"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>16</v>
       </c>
+      <c r="E39" s="11"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="18"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G39" s="4"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="3"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="E40" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="18"/>
-    </row>
-    <row r="41" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G40" s="4"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="3"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="18"/>
-    </row>
-    <row r="42" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G41" s="1"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="3"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="18"/>
-    </row>
-    <row r="43" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G42" s="4"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="25"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="9">
+      <c r="F43" s="9">
         <v>75</v>
       </c>
-      <c r="I43" s="19"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H43" s="19"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="18"/>
+    </row>
+    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>28</v>
       </c>
@@ -2251,19 +2207,18 @@
       <c r="C44" s="9">
         <v>200</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="14" t="s">
+      <c r="D44" s="14" t="s">
         <v>30</v>
       </c>
+      <c r="E44" s="11"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="18"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="5"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="18"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>31</v>
       </c>
@@ -2273,23 +2228,22 @@
       <c r="C45" s="9">
         <v>195</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G45" s="3">
+      <c r="F45" s="3">
         <v>20</v>
       </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G45" s="1"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="18"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>33</v>
       </c>
@@ -2299,23 +2253,22 @@
       <c r="C46" s="9">
         <v>195</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G46" s="9">
+      <c r="F46" s="9">
         <v>10</v>
       </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G46" s="1"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="18"/>
+    </row>
+    <row r="47" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>35</v>
       </c>
@@ -2325,41 +2278,39 @@
       <c r="C47" s="9">
         <v>295</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="14" t="s">
+      <c r="D47" s="14" t="s">
         <v>36</v>
       </c>
+      <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="18"/>
-    </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G47" s="1"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="18"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="3">
+      <c r="F48" s="3">
         <v>20</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G48" s="1"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="18"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>40</v>
       </c>
@@ -2369,23 +2320,22 @@
       <c r="C49" s="3">
         <v>255</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G49" s="3">
+      <c r="F49" s="3">
         <v>50</v>
       </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G49" s="5"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="18"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>44</v>
       </c>
@@ -2395,23 +2345,22 @@
       <c r="C50" s="3">
         <v>260</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G50" s="3">
+      <c r="F50" s="3">
         <v>50</v>
       </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="18"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="18"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>46</v>
       </c>
@@ -2421,23 +2370,22 @@
       <c r="C51" s="3">
         <v>295</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="3">
+      <c r="F51" s="3">
         <v>20</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="18"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G51" s="1"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="18"/>
+    </row>
+    <row r="52" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>48</v>
       </c>
@@ -2447,23 +2395,22 @@
       <c r="C52" s="3">
         <v>270</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="3">
+      <c r="F52" s="3">
         <v>50</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="18"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G52" s="1"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="18"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>50</v>
       </c>
@@ -2473,23 +2420,22 @@
       <c r="C53" s="3">
         <v>255</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G53" s="3">
+      <c r="F53" s="3">
         <v>50</v>
       </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="18"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G53" s="1"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="18"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2499,39 +2445,37 @@
       <c r="C54" s="3">
         <v>295</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G54" s="3">
+      <c r="F54" s="3">
         <v>20</v>
       </c>
-      <c r="H54" s="1"/>
-      <c r="I54" s="19"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-    </row>
-    <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="55" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="27"/>
       <c r="C55" s="26"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="19"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-    </row>
-    <row r="56" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>55</v>
       </c>
@@ -2541,17 +2485,16 @@
       <c r="C56" s="3">
         <v>250</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="19"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-    </row>
-    <row r="57" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>56</v>
       </c>
@@ -2561,17 +2504,16 @@
       <c r="C57" s="3">
         <v>180</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="19"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-    </row>
-    <row r="58" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>57</v>
       </c>
@@ -2581,17 +2523,16 @@
       <c r="C58" s="3">
         <v>195</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="19"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-    </row>
-    <row r="59" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>58</v>
       </c>
@@ -2601,17 +2542,16 @@
       <c r="C59" s="3">
         <v>265</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="19"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="18"/>
       <c r="J59" s="18"/>
       <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-    </row>
-    <row r="60" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="75" t="s">
         <v>59</v>
       </c>
@@ -2620,14 +2560,13 @@
       <c r="D60" s="75"/>
       <c r="E60" s="75"/>
       <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="19"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="18"/>
       <c r="J60" s="18"/>
       <c r="K60" s="18"/>
-      <c r="L60" s="18"/>
-    </row>
-    <row r="61" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="76" t="s">
         <v>60</v>
       </c>
@@ -2636,78 +2575,74 @@
       <c r="D61" s="76"/>
       <c r="E61" s="76"/>
       <c r="F61" s="76"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="18"/>
       <c r="I61" s="18"/>
       <c r="J61" s="18"/>
       <c r="K61" s="18"/>
-      <c r="L61" s="18"/>
-    </row>
-    <row r="62" spans="1:12" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="28"/>
       <c r="B62" s="28"/>
       <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
+      <c r="D62" s="30"/>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="18"/>
       <c r="I62" s="18"/>
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
-    </row>
-    <row r="63" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="28"/>
       <c r="B63" s="28"/>
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
       <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
+      <c r="H63" s="18"/>
       <c r="I63" s="18"/>
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
-      <c r="L63" s="18"/>
-    </row>
-    <row r="64" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="28"/>
       <c r="B64" s="28"/>
       <c r="C64" s="28"/>
       <c r="D64" s="28"/>
       <c r="E64" s="28"/>
       <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
+      <c r="H64" s="18"/>
       <c r="I64" s="18"/>
       <c r="J64" s="18"/>
       <c r="K64" s="18"/>
-      <c r="L64" s="18"/>
-    </row>
-    <row r="65" spans="9:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="8:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H65" s="18"/>
       <c r="I65" s="18"/>
       <c r="J65" s="18"/>
       <c r="K65" s="18"/>
-      <c r="L65" s="18"/>
-    </row>
-    <row r="66" spans="9:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="8:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H66" s="18"/>
       <c r="I66" s="18"/>
       <c r="J66" s="18"/>
       <c r="K66" s="18"/>
-      <c r="L66" s="18"/>
-    </row>
-    <row r="67" spans="9:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="67" spans="8:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E31:G38">
-    <sortCondition ref="E31:E38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D31:F38">
+    <sortCondition ref="D31:D38"/>
   </sortState>
   <mergeCells count="7">
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0" bottom="0" header="0.11811023622047249" footer="0.11811023622047249"/>
   <pageSetup paperSize="9" scale="75" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2719,8 +2654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3160,7 +3095,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3399,57 +3334,57 @@
     </row>
     <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
+        <f>Касса!E7</f>
+        <v>0</v>
+      </c>
+      <c r="B20" s="45">
+        <f>Касса!D7</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="46">
         <f>Касса!F7</f>
-        <v>0</v>
-      </c>
-      <c r="B20" s="45">
-        <f>Касса!E7</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="46">
-        <f>Касса!G7</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
+        <f>Касса!E8</f>
+        <v>0</v>
+      </c>
+      <c r="B21" s="45">
+        <f>Касса!D8</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="46">
         <f>Касса!F8</f>
-        <v>0</v>
-      </c>
-      <c r="B21" s="45">
-        <f>Касса!E8</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="46">
-        <f>Касса!G8</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
+        <f>Касса!E9</f>
+        <v>0</v>
+      </c>
+      <c r="B22" s="45">
+        <f>Касса!D9</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="46">
         <f>Касса!F9</f>
-        <v>0</v>
-      </c>
-      <c r="B22" s="45">
-        <f>Касса!E9</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="46">
-        <f>Касса!G9</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
+        <f>Касса!E10</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="45">
+        <f>Касса!D10</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="46">
         <f>Касса!F10</f>
-        <v>0</v>
-      </c>
-      <c r="B23" s="45">
-        <f>Касса!E10</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="46">
-        <f>Касса!G10</f>
         <v>0</v>
       </c>
     </row>
@@ -3462,85 +3397,85 @@
     </row>
     <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
+        <f>Касса!E12</f>
+        <v>0</v>
+      </c>
+      <c r="B25" s="45">
+        <f>Касса!D12</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="46">
         <f>Касса!F12</f>
-        <v>0</v>
-      </c>
-      <c r="B25" s="45">
-        <f>Касса!E12</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="46">
-        <f>Касса!G12</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
+        <f>Касса!E13</f>
+        <v>0</v>
+      </c>
+      <c r="B26" s="45">
+        <f>Касса!D13</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="46">
         <f>Касса!F13</f>
-        <v>0</v>
-      </c>
-      <c r="B26" s="45">
-        <f>Касса!E13</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="46">
-        <f>Касса!G13</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
+        <f>Касса!E14</f>
+        <v>0</v>
+      </c>
+      <c r="B27" s="45">
+        <f>Касса!D14</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="46">
         <f>Касса!F14</f>
-        <v>0</v>
-      </c>
-      <c r="B27" s="45">
-        <f>Касса!E14</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="46">
-        <f>Касса!G14</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
+        <f>Касса!E15</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="45">
+        <f>Касса!D15</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="46">
         <f>Касса!F15</f>
-        <v>0</v>
-      </c>
-      <c r="B28" s="45">
-        <f>Касса!E15</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="46">
-        <f>Касса!G15</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
+        <f>Касса!E16</f>
+        <v>0</v>
+      </c>
+      <c r="B29" s="45">
+        <f>Касса!D16</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="46">
         <f>Касса!F16</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="45">
-        <f>Касса!E16</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="46">
-        <f>Касса!G16</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
+        <f>Касса!E17</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="45">
+        <f>Касса!D17</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="46">
         <f>Касса!F17</f>
-        <v>0</v>
-      </c>
-      <c r="B30" s="45">
-        <f>Касса!E17</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="46">
-        <f>Касса!G17</f>
         <v>0</v>
       </c>
     </row>
@@ -3553,85 +3488,85 @@
     </row>
     <row r="32" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
+        <f>Касса!E19</f>
+        <v>0</v>
+      </c>
+      <c r="B32" s="45">
+        <f>Касса!D19</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="46">
         <f>Касса!F19</f>
-        <v>0</v>
-      </c>
-      <c r="B32" s="45">
-        <f>Касса!E19</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="46">
-        <f>Касса!G19</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
+        <f>Касса!E20</f>
+        <v>0</v>
+      </c>
+      <c r="B33" s="45">
+        <f>Касса!D20</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="46">
         <f>Касса!F20</f>
-        <v>0</v>
-      </c>
-      <c r="B33" s="45">
-        <f>Касса!E20</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="46">
-        <f>Касса!G20</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
+        <f>Касса!E21</f>
+        <v>0</v>
+      </c>
+      <c r="B34" s="45">
+        <f>Касса!D21</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="46">
         <f>Касса!F21</f>
-        <v>0</v>
-      </c>
-      <c r="B34" s="45">
-        <f>Касса!E21</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="46">
-        <f>Касса!G21</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
+        <f>Касса!E22</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="45">
+        <f>Касса!D22</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="46">
         <f>Касса!F22</f>
-        <v>0</v>
-      </c>
-      <c r="B35" s="45">
-        <f>Касса!E22</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="46">
-        <f>Касса!G22</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
+        <f>Касса!E23</f>
+        <v>0</v>
+      </c>
+      <c r="B36" s="45">
+        <f>Касса!D23</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="46">
         <f>Касса!F23</f>
-        <v>0</v>
-      </c>
-      <c r="B36" s="45">
-        <f>Касса!E23</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="46">
-        <f>Касса!G23</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
+        <f>Касса!E24</f>
+        <v>0</v>
+      </c>
+      <c r="B37" s="45">
+        <f>Касса!D24</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="46">
         <f>Касса!F24</f>
-        <v>0</v>
-      </c>
-      <c r="B37" s="45">
-        <f>Касса!E24</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="46">
-        <f>Касса!G24</f>
         <v>0</v>
       </c>
     </row>
@@ -3644,57 +3579,57 @@
     </row>
     <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="38">
+        <f>Касса!E26</f>
+        <v>0</v>
+      </c>
+      <c r="B39" s="45">
+        <f>Касса!D26</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="46">
         <f>Касса!F26</f>
-        <v>0</v>
-      </c>
-      <c r="B39" s="45">
-        <f>Касса!E26</f>
-        <v>0</v>
-      </c>
-      <c r="C39" s="46">
-        <f>Касса!G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="38">
+        <f>Касса!E27</f>
+        <v>0</v>
+      </c>
+      <c r="B40" s="45">
+        <f>Касса!D27</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="46">
         <f>Касса!F27</f>
-        <v>0</v>
-      </c>
-      <c r="B40" s="45">
-        <f>Касса!E27</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="46">
-        <f>Касса!G27</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="38">
+        <f>Касса!E28</f>
+        <v>0</v>
+      </c>
+      <c r="B41" s="45">
+        <f>Касса!D28</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="46">
         <f>Касса!F28</f>
-        <v>0</v>
-      </c>
-      <c r="B41" s="45">
-        <f>Касса!E28</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="46">
-        <f>Касса!G28</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
+        <f>Касса!E29</f>
+        <v>0</v>
+      </c>
+      <c r="B42" s="45">
+        <f>Касса!D29</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="46">
         <f>Касса!F29</f>
-        <v>0</v>
-      </c>
-      <c r="B42" s="45">
-        <f>Касса!E29</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="46">
-        <f>Касса!G29</f>
         <v>0</v>
       </c>
     </row>
@@ -3707,113 +3642,113 @@
     </row>
     <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="38">
+        <f>Касса!E31</f>
+        <v>0</v>
+      </c>
+      <c r="B44" s="45">
+        <f>Касса!D31</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="46">
         <f>Касса!F31</f>
-        <v>0</v>
-      </c>
-      <c r="B44" s="45">
-        <f>Касса!E31</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="46">
-        <f>Касса!G31</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="38">
+        <f>Касса!E32</f>
+        <v>0</v>
+      </c>
+      <c r="B45" s="45">
+        <f>Касса!D32</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="46">
         <f>Касса!F32</f>
-        <v>0</v>
-      </c>
-      <c r="B45" s="45">
-        <f>Касса!E32</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="46">
-        <f>Касса!G32</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="38">
+        <f>Касса!E33</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="45">
+        <f>Касса!D33</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="46">
         <f>Касса!F33</f>
-        <v>0</v>
-      </c>
-      <c r="B46" s="45">
-        <f>Касса!E33</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="46">
-        <f>Касса!G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="38">
+        <f>Касса!E34</f>
+        <v>0</v>
+      </c>
+      <c r="B47" s="45">
+        <f>Касса!D34</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="46">
         <f>Касса!F34</f>
-        <v>0</v>
-      </c>
-      <c r="B47" s="45">
-        <f>Касса!E34</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="46">
-        <f>Касса!G34</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="38">
+        <f>Касса!E35</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="45">
+        <f>Касса!D35</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="46">
         <f>Касса!F35</f>
-        <v>0</v>
-      </c>
-      <c r="B48" s="45">
-        <f>Касса!E35</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="46">
-        <f>Касса!G35</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
+        <f>Касса!E36</f>
+        <v>0</v>
+      </c>
+      <c r="B49" s="45">
+        <f>Касса!D36</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="46">
         <f>Касса!F36</f>
-        <v>0</v>
-      </c>
-      <c r="B49" s="45">
-        <f>Касса!E36</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="46">
-        <f>Касса!G36</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="38">
+        <f>Касса!E37</f>
+        <v>0</v>
+      </c>
+      <c r="B50" s="45">
+        <f>Касса!D37</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="46">
         <f>Касса!F37</f>
-        <v>0</v>
-      </c>
-      <c r="B50" s="45">
-        <f>Касса!E37</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="46">
-        <f>Касса!G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="38">
+        <f>Касса!E38</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="45">
+        <f>Касса!D38</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="46">
         <f>Касса!F38</f>
-        <v>0</v>
-      </c>
-      <c r="B51" s="45">
-        <f>Касса!E38</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="46">
-        <f>Касса!G38</f>
         <v>0</v>
       </c>
     </row>
@@ -4001,7 +3936,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="11"/>
       <c r="E7" s="6">
-        <f>Касса!E7</f>
+        <f>Касса!D7</f>
         <v>0</v>
       </c>
       <c r="F7" s="3"/>
@@ -4021,7 +3956,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="11"/>
       <c r="E8" s="6">
-        <f>Касса!E8</f>
+        <f>Касса!D8</f>
         <v>0</v>
       </c>
       <c r="F8" s="3"/>
@@ -4041,7 +3976,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="11"/>
       <c r="E9" s="6">
-        <f>Касса!E9</f>
+        <f>Касса!D9</f>
         <v>0</v>
       </c>
       <c r="F9" s="3"/>
@@ -4061,7 +3996,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6">
-        <f>Касса!E10</f>
+        <f>Касса!D10</f>
         <v>0</v>
       </c>
       <c r="F10" s="3"/>
@@ -4100,7 +4035,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="11"/>
       <c r="E12" s="6">
-        <f>Касса!E12</f>
+        <f>Касса!D12</f>
         <v>0</v>
       </c>
       <c r="F12" s="3"/>
@@ -4120,7 +4055,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="11"/>
       <c r="E13" s="6">
-        <f>Касса!E13</f>
+        <f>Касса!D13</f>
         <v>0</v>
       </c>
       <c r="F13" s="3"/>
@@ -4140,7 +4075,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6">
-        <f>Касса!E14</f>
+        <f>Касса!D14</f>
         <v>0</v>
       </c>
       <c r="F14" s="3"/>
@@ -4160,7 +4095,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="11"/>
       <c r="E15" s="6">
-        <f>Касса!E15</f>
+        <f>Касса!D15</f>
         <v>0</v>
       </c>
       <c r="F15" s="3"/>
@@ -4180,7 +4115,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="11"/>
       <c r="E16" s="6">
-        <f>Касса!E16</f>
+        <f>Касса!D16</f>
         <v>0</v>
       </c>
       <c r="F16" s="3"/>
@@ -4200,7 +4135,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="11"/>
       <c r="E17" s="6">
-        <f>Касса!E17</f>
+        <f>Касса!D17</f>
         <v>0</v>
       </c>
       <c r="F17" s="3"/>
@@ -4239,7 +4174,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="17"/>
       <c r="E19" s="10">
-        <f>Касса!E19</f>
+        <f>Касса!D19</f>
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
@@ -4259,7 +4194,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="11"/>
       <c r="E20" s="10">
-        <f>Касса!E20</f>
+        <f>Касса!D20</f>
         <v>0</v>
       </c>
       <c r="F20" s="3"/>
@@ -4279,7 +4214,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="11"/>
       <c r="E21" s="10">
-        <f>Касса!E21</f>
+        <f>Касса!D21</f>
         <v>0</v>
       </c>
       <c r="F21" s="3"/>
@@ -4299,7 +4234,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10">
-        <f>Касса!E22</f>
+        <f>Касса!D22</f>
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
@@ -4319,7 +4254,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10">
-        <f>Касса!E23</f>
+        <f>Касса!D23</f>
         <v>0</v>
       </c>
       <c r="F23" s="3"/>
@@ -4339,7 +4274,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10">
-        <f>Касса!E24</f>
+        <f>Касса!D24</f>
         <v>0</v>
       </c>
       <c r="F24" s="3"/>
@@ -4378,7 +4313,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="11"/>
       <c r="E26" s="16">
-        <f>Касса!E26</f>
+        <f>Касса!D26</f>
         <v>0</v>
       </c>
       <c r="F26" s="3"/>
@@ -4398,7 +4333,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="11"/>
       <c r="E27" s="16">
-        <f>Касса!E27</f>
+        <f>Касса!D27</f>
         <v>0</v>
       </c>
       <c r="F27" s="3"/>
@@ -4418,7 +4353,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="11"/>
       <c r="E28" s="16">
-        <f>Касса!E28</f>
+        <f>Касса!D28</f>
         <v>0</v>
       </c>
       <c r="F28" s="3"/>
@@ -4438,7 +4373,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="11"/>
       <c r="E29" s="16">
-        <f>Касса!E29</f>
+        <f>Касса!D29</f>
         <v>0</v>
       </c>
       <c r="F29" s="3"/>
@@ -4471,7 +4406,7 @@
       <c r="C31" s="54"/>
       <c r="D31" s="11"/>
       <c r="E31" s="6">
-        <f>Касса!E31</f>
+        <f>Касса!D31</f>
         <v>0</v>
       </c>
       <c r="F31" s="3"/>
@@ -4488,7 +4423,7 @@
       <c r="C32" s="54"/>
       <c r="D32" s="11"/>
       <c r="E32" s="6">
-        <f>Касса!E32</f>
+        <f>Касса!D32</f>
         <v>0</v>
       </c>
       <c r="F32" s="3"/>
@@ -4505,7 +4440,7 @@
       <c r="C33" s="54"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6">
-        <f>Касса!E33</f>
+        <f>Касса!D33</f>
         <v>0</v>
       </c>
       <c r="F33" s="3"/>
@@ -4522,7 +4457,7 @@
       <c r="C34" s="54"/>
       <c r="D34" s="11"/>
       <c r="E34" s="6">
-        <f>Касса!E34</f>
+        <f>Касса!D34</f>
         <v>0</v>
       </c>
       <c r="F34" s="3"/>
@@ -4539,7 +4474,7 @@
       <c r="C35" s="54"/>
       <c r="D35" s="11"/>
       <c r="E35" s="6">
-        <f>Касса!E35</f>
+        <f>Касса!D35</f>
         <v>0</v>
       </c>
       <c r="F35" s="3"/>
@@ -4556,7 +4491,7 @@
       <c r="C36" s="54"/>
       <c r="D36" s="11"/>
       <c r="E36" s="6">
-        <f>Касса!E36</f>
+        <f>Касса!D36</f>
         <v>0</v>
       </c>
       <c r="F36" s="3"/>
@@ -4573,7 +4508,7 @@
       <c r="C37" s="54"/>
       <c r="D37" s="11"/>
       <c r="E37" s="6">
-        <f>Касса!E37</f>
+        <f>Касса!D37</f>
         <v>0</v>
       </c>
       <c r="F37" s="3"/>
@@ -4590,7 +4525,7 @@
       <c r="C38" s="54"/>
       <c r="D38" s="11"/>
       <c r="E38" s="6">
-        <f>Касса!E38</f>
+        <f>Касса!D38</f>
         <v>0</v>
       </c>
       <c r="F38" s="3"/>
@@ -5664,7 +5599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -5786,7 +5721,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="11"/>
       <c r="E7" s="6">
-        <f>Касса!E7</f>
+        <f>Касса!D7</f>
         <v>0</v>
       </c>
       <c r="F7" s="3"/>
@@ -5806,7 +5741,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="11"/>
       <c r="E8" s="6">
-        <f>Касса!E8</f>
+        <f>Касса!D8</f>
         <v>0</v>
       </c>
       <c r="F8" s="3"/>
@@ -5826,7 +5761,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="11"/>
       <c r="E9" s="6">
-        <f>Касса!E9</f>
+        <f>Касса!D9</f>
         <v>0</v>
       </c>
       <c r="F9" s="3"/>
@@ -5846,7 +5781,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="11"/>
       <c r="E10" s="6">
-        <f>Касса!E10</f>
+        <f>Касса!D10</f>
         <v>0</v>
       </c>
       <c r="F10" s="3"/>
@@ -5885,7 +5820,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="11"/>
       <c r="E12" s="6">
-        <f>Касса!E12</f>
+        <f>Касса!D12</f>
         <v>0</v>
       </c>
       <c r="F12" s="3"/>
@@ -5905,7 +5840,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="11"/>
       <c r="E13" s="6">
-        <f>Касса!E13</f>
+        <f>Касса!D13</f>
         <v>0</v>
       </c>
       <c r="F13" s="3"/>
@@ -5925,7 +5860,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="11"/>
       <c r="E14" s="6">
-        <f>Касса!E14</f>
+        <f>Касса!D14</f>
         <v>0</v>
       </c>
       <c r="F14" s="3"/>
@@ -5945,7 +5880,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="11"/>
       <c r="E15" s="6">
-        <f>Касса!E15</f>
+        <f>Касса!D15</f>
         <v>0</v>
       </c>
       <c r="F15" s="3"/>
@@ -5965,7 +5900,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="11"/>
       <c r="E16" s="6">
-        <f>Касса!E16</f>
+        <f>Касса!D16</f>
         <v>0</v>
       </c>
       <c r="F16" s="3"/>
@@ -5985,7 +5920,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="11"/>
       <c r="E17" s="6">
-        <f>Касса!E17</f>
+        <f>Касса!D17</f>
         <v>0</v>
       </c>
       <c r="F17" s="3"/>
@@ -6024,7 +5959,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="17"/>
       <c r="E19" s="10">
-        <f>Касса!E19</f>
+        <f>Касса!D19</f>
         <v>0</v>
       </c>
       <c r="F19" s="3"/>
@@ -6044,7 +5979,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="11"/>
       <c r="E20" s="10">
-        <f>Касса!E20</f>
+        <f>Касса!D20</f>
         <v>0</v>
       </c>
       <c r="F20" s="3"/>
@@ -6064,7 +5999,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="11"/>
       <c r="E21" s="10">
-        <f>Касса!E21</f>
+        <f>Касса!D21</f>
         <v>0</v>
       </c>
       <c r="F21" s="3"/>
@@ -6084,7 +6019,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10">
-        <f>Касса!E22</f>
+        <f>Касса!D22</f>
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
@@ -6104,7 +6039,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="11"/>
       <c r="E23" s="10">
-        <f>Касса!E23</f>
+        <f>Касса!D23</f>
         <v>0</v>
       </c>
       <c r="F23" s="3"/>
@@ -6124,7 +6059,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10">
-        <f>Касса!E24</f>
+        <f>Касса!D24</f>
         <v>0</v>
       </c>
       <c r="F24" s="3"/>
@@ -6163,7 +6098,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="11"/>
       <c r="E26" s="16">
-        <f>Касса!E26</f>
+        <f>Касса!D26</f>
         <v>0</v>
       </c>
       <c r="F26" s="3"/>
@@ -6183,7 +6118,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="11"/>
       <c r="E27" s="16">
-        <f>Касса!E27</f>
+        <f>Касса!D27</f>
         <v>0</v>
       </c>
       <c r="F27" s="3"/>
@@ -6203,7 +6138,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="11"/>
       <c r="E28" s="16">
-        <f>Касса!E28</f>
+        <f>Касса!D28</f>
         <v>0</v>
       </c>
       <c r="F28" s="3"/>
@@ -6223,7 +6158,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="11"/>
       <c r="E29" s="16">
-        <f>Касса!E29</f>
+        <f>Касса!D29</f>
         <v>0</v>
       </c>
       <c r="F29" s="3"/>
@@ -6261,7 +6196,7 @@
       <c r="C31" s="9"/>
       <c r="D31" s="11"/>
       <c r="E31" s="6">
-        <f>Касса!E31</f>
+        <f>Касса!D31</f>
         <v>0</v>
       </c>
       <c r="F31" s="3"/>
@@ -6281,7 +6216,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="11"/>
       <c r="E32" s="6">
-        <f>Касса!E32</f>
+        <f>Касса!D32</f>
         <v>0</v>
       </c>
       <c r="F32" s="3"/>
@@ -6301,7 +6236,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="11"/>
       <c r="E33" s="6">
-        <f>Касса!E33</f>
+        <f>Касса!D33</f>
         <v>0</v>
       </c>
       <c r="F33" s="3"/>
@@ -6321,7 +6256,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="11"/>
       <c r="E34" s="6">
-        <f>Касса!E34</f>
+        <f>Касса!D34</f>
         <v>0</v>
       </c>
       <c r="F34" s="3"/>
@@ -6341,7 +6276,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="6">
-        <f>Касса!E35</f>
+        <f>Касса!D35</f>
         <v>0</v>
       </c>
       <c r="F35" s="3"/>
@@ -6361,7 +6296,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="11"/>
       <c r="E36" s="6">
-        <f>Касса!E36</f>
+        <f>Касса!D36</f>
         <v>0</v>
       </c>
       <c r="F36" s="3"/>
@@ -6381,7 +6316,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="11"/>
       <c r="E37" s="6">
-        <f>Касса!E37</f>
+        <f>Касса!D37</f>
         <v>0</v>
       </c>
       <c r="F37" s="3"/>
@@ -6401,7 +6336,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="11"/>
       <c r="E38" s="6">
-        <f>Касса!E38</f>
+        <f>Касса!D38</f>
         <v>0</v>
       </c>
       <c r="F38" s="3"/>

</xml_diff>

<commit_message>
template: enforce breakfasts into column A and limit to before 'САЛАТЫ И ХОЛОДНЫЕ ЗАКУСКИ'; add variant splitting for names/weights/prices (e.g., 'Омлет/Омлет с брокколи', 'Яйцо отварное/жареное'); tests green
</commit_message>
<xml_diff>
--- a/excel_menu_gui/templates/Шаблон меню пример.xlsx
+++ b/excel_menu_gui/templates/Шаблон меню пример.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katya\Desktop\menurepit\excel_menu_gui\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5DCD69-2003-490B-886C-3057B8DE5114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61775D3-E71F-4CDF-AF4A-77D91032EEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="447" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="447" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Касса" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
     <sheet name="Раздача" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Завтрак!$A$1:$C$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Завтрак!$A$1:$C$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Обед!$A$1:$G$66</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Раздача!$A$1:$G$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Хц!$A$1:$G$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Хц!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
   <si>
     <t xml:space="preserve">Утверждаю </t>
   </si>
@@ -125,9 +125,6 @@
     <t>Чай фруктовый в ассортименте</t>
   </si>
   <si>
-    <t>225 мл</t>
-  </si>
-  <si>
     <t>Сэндвич с бужениной</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t xml:space="preserve">                                                           г.Москва,Овчинниковская наб.,д.18/1,стр.2</t>
   </si>
   <si>
-    <t>200/300</t>
-  </si>
-  <si>
     <t>Выходы</t>
   </si>
   <si>
@@ -276,6 +270,9 @@
   </si>
   <si>
     <t>1 сентября</t>
+  </si>
+  <si>
+    <t>225мл</t>
   </si>
 </sst>
 </file>
@@ -565,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -606,13 +603,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -780,7 +790,6 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,6 +846,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1544,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1571,28 +1586,28 @@
     </row>
     <row r="2" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="79" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="80" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="77" t="s">
+      <c r="B3" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="77"/>
+      <c r="D3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1609,14 +1624,14 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
       <c r="G5" s="1"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -1649,7 +1664,7 @@
       <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="73"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="6"/>
@@ -1696,9 +1711,9 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="19"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="66"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="65"/>
       <c r="L10" s="60"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
@@ -1715,16 +1730,16 @@
       <c r="F11" s="11"/>
       <c r="G11" s="4"/>
       <c r="H11" s="19"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="66"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="60"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="73"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
@@ -1732,16 +1747,16 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="66"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="65"/>
       <c r="L12" s="60"/>
       <c r="M12" s="60"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
     </row>
     <row r="13" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="73"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6"/>
@@ -1749,9 +1764,9 @@
       <c r="F13" s="3"/>
       <c r="G13" s="1"/>
       <c r="H13" s="19"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="66"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="65"/>
       <c r="L13" s="60"/>
       <c r="M13" s="60"/>
       <c r="N13" s="60"/>
@@ -1766,9 +1781,9 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="66"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="65"/>
       <c r="L14" s="60"/>
       <c r="M14" s="60"/>
       <c r="N14" s="60"/>
@@ -1783,12 +1798,12 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
       <c r="O15" s="60"/>
     </row>
     <row r="16" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1800,9 +1815,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="66"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="65"/>
       <c r="L16" s="60"/>
       <c r="M16" s="60"/>
       <c r="N16" s="60"/>
@@ -1838,12 +1853,12 @@
       <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="74"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="71"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
@@ -1851,7 +1866,7 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="74"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="10"/>
@@ -1864,7 +1879,7 @@
       <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="6"/>
@@ -1944,7 +1959,7 @@
       <c r="K26" s="18"/>
     </row>
     <row r="27" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="74"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="6"/>
@@ -1957,7 +1972,7 @@
       <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="74"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="10"/>
@@ -1970,7 +1985,9 @@
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="10"/>
@@ -1983,9 +2000,7 @@
       <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="14" t="s">
@@ -2009,9 +2024,9 @@
       <c r="G31" s="19"/>
       <c r="H31" s="20"/>
       <c r="I31" s="18"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="70"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="69"/>
     </row>
     <row r="32" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
@@ -2023,8 +2038,8 @@
       <c r="G32" s="19"/>
       <c r="H32" s="20"/>
       <c r="I32" s="18"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="65"/>
       <c r="L32" s="60"/>
     </row>
     <row r="33" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2187,10 +2202,10 @@
         <v>26</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="F43" s="9">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="18"/>
@@ -2199,16 +2214,16 @@
     </row>
     <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C44" s="9">
         <v>200</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
@@ -2220,19 +2235,19 @@
     </row>
     <row r="45" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="9">
         <v>195</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F45" s="3">
         <v>20</v>
@@ -2245,19 +2260,19 @@
     </row>
     <row r="46" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="9">
         <v>195</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F46" s="9">
         <v>10</v>
@@ -2270,16 +2285,16 @@
     </row>
     <row r="47" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="9">
         <v>295</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -2291,15 +2306,15 @@
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
       <c r="D48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F48" s="3">
         <v>20</v>
@@ -2312,19 +2327,19 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C49" s="3">
         <v>255</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="F49" s="3">
         <v>50</v>
@@ -2337,19 +2352,19 @@
     </row>
     <row r="50" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50" s="3">
         <v>260</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="3">
         <v>50</v>
@@ -2362,19 +2377,19 @@
     </row>
     <row r="51" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="3">
         <v>295</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" s="3">
         <v>20</v>
@@ -2387,16 +2402,16 @@
     </row>
     <row r="52" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52" s="3">
         <v>270</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>10</v>
@@ -2412,16 +2427,16 @@
     </row>
     <row r="53" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C53" s="3">
         <v>255</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>10</v>
@@ -2437,19 +2452,19 @@
     </row>
     <row r="54" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" s="3">
         <v>295</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F54" s="3">
         <v>20</v>
@@ -2462,7 +2477,7 @@
     </row>
     <row r="55" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="27"/>
       <c r="C55" s="26"/>
@@ -2477,7 +2492,7 @@
     </row>
     <row r="56" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -2496,7 +2511,7 @@
     </row>
     <row r="57" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>12</v>
@@ -2515,7 +2530,7 @@
     </row>
     <row r="58" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
@@ -2534,7 +2549,7 @@
     </row>
     <row r="59" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
@@ -2552,14 +2567,14 @@
       <c r="K59" s="18"/>
     </row>
     <row r="60" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
+      <c r="A60" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="74"/>
+      <c r="C60" s="74"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="74"/>
       <c r="G60" s="1"/>
       <c r="H60" s="19"/>
       <c r="I60" s="18"/>
@@ -2567,14 +2582,14 @@
       <c r="K60" s="18"/>
     </row>
     <row r="61" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="76"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
+      <c r="A61" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="75"/>
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="75"/>
+      <c r="F61" s="75"/>
       <c r="G61" s="1"/>
       <c r="H61" s="18"/>
       <c r="I61" s="18"/>
@@ -2654,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2685,23 +2700,23 @@
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="78"/>
+      <c r="B3" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="77"/>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="29"/>
@@ -2712,7 +2727,7 @@
         <v>Вес/ед.изм.</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="36" t="str">
         <f>Касса!C6</f>
@@ -3028,18 +3043,9 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38">
-        <f>Касса!B29</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="39">
-        <f>Касса!A29</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="40">
-        <f>Касса!C29</f>
-        <v>0</v>
-      </c>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
     </row>
     <row r="30" spans="1:3" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38"/>
@@ -3047,41 +3053,37 @@
       <c r="C30" s="40"/>
     </row>
     <row r="31" spans="1:3" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="81" t="str">
+        <f>Касса!A60</f>
+        <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
+      </c>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="82" t="str">
-        <f>Касса!A60</f>
-        <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
-      </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
-    </row>
-    <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="83" t="str">
         <f>Касса!A61</f>
         <v>Блюда могут содержать следы молочных продуктов, яичных продуктов, рыбы, моллюсков, кунжута, горчицы, сои, злаков, содержащих глютен, арахиса, аспартама, диоксида серы и сульфатов, люпина, орехов, ракообразных, сельдерея. Допускается использовать аналогичные указанным компоненты, отечественного или импортного производства, соответствующие нормативным и правовым документам Российской Федерации и Таможенного союза.</v>
       </c>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+    </row>
+    <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
     </row>
     <row r="34" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-    </row>
-    <row r="35" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-    </row>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+    </row>
+    <row r="35" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C35"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C34"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3092,10 +3094,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3119,29 +3121,29 @@
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="71" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="72" t="s">
-        <v>61</v>
+      <c r="C3" s="71" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="31"/>
-      <c r="C4" s="72" t="s">
-        <v>63</v>
+      <c r="C4" s="71" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="41"/>
       <c r="C5" s="29"/>
@@ -3159,658 +3161,678 @@
     </row>
     <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <f>Касса!B31</f>
+        <f>Касса!B30</f>
         <v>0</v>
       </c>
       <c r="B7" s="45">
-        <f>Касса!A31</f>
+        <f>Касса!A30</f>
         <v>0</v>
       </c>
       <c r="C7" s="46">
-        <f>Касса!C31</f>
+        <f>Касса!C30</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <f>Касса!B32</f>
+        <f>Касса!B31</f>
         <v>0</v>
       </c>
       <c r="B8" s="45">
-        <f>Касса!A32</f>
+        <f>Касса!A31</f>
         <v>0</v>
       </c>
       <c r="C8" s="46">
-        <f>Касса!C32</f>
+        <f>Касса!C31</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <f>Касса!B33</f>
+        <f>Касса!B32</f>
         <v>0</v>
       </c>
       <c r="B9" s="45">
-        <f>Касса!A33</f>
+        <f>Касса!A32</f>
         <v>0</v>
       </c>
       <c r="C9" s="46">
-        <f>Касса!C33</f>
+        <f>Касса!C32</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
-        <f>Касса!B34</f>
+        <f>Касса!B33</f>
         <v>0</v>
       </c>
       <c r="B10" s="45">
-        <f>Касса!A34</f>
+        <f>Касса!A33</f>
         <v>0</v>
       </c>
       <c r="C10" s="46">
-        <f>Касса!C34</f>
+        <f>Касса!C33</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
-        <f>Касса!B35</f>
+        <f>Касса!B34</f>
         <v>0</v>
       </c>
       <c r="B11" s="45">
-        <f>Касса!A35</f>
+        <f>Касса!A34</f>
         <v>0</v>
       </c>
       <c r="C11" s="46">
-        <f>Касса!C35</f>
+        <f>Касса!C34</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
-        <f>Касса!B36</f>
+        <f>Касса!B35</f>
         <v>0</v>
       </c>
       <c r="B12" s="45">
-        <f>Касса!A36</f>
+        <f>Касса!A35</f>
         <v>0</v>
       </c>
       <c r="C12" s="46">
-        <f>Касса!C36</f>
+        <f>Касса!C35</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
-        <f>Касса!B37</f>
+        <f>Касса!B36</f>
         <v>0</v>
       </c>
       <c r="B13" s="45">
-        <f>Касса!A37</f>
+        <f>Касса!A36</f>
         <v>0</v>
       </c>
       <c r="C13" s="46">
-        <f>Касса!C37</f>
+        <f>Касса!C36</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <f>Касса!B38</f>
+        <f>Касса!B37</f>
         <v>0</v>
       </c>
       <c r="B14" s="45">
-        <f>Касса!A38</f>
+        <f>Касса!A37</f>
         <v>0</v>
       </c>
       <c r="C14" s="46">
-        <f>Касса!C38</f>
+        <f>Касса!C37</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
-        <f>Касса!B39</f>
+        <f>Касса!B38</f>
         <v>0</v>
       </c>
       <c r="B15" s="45">
-        <f>Касса!A39</f>
+        <f>Касса!A38</f>
         <v>0</v>
       </c>
       <c r="C15" s="46">
-        <f>Касса!C39</f>
+        <f>Касса!C38</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
-        <f>Касса!B40</f>
+        <f>Касса!B39</f>
         <v>0</v>
       </c>
       <c r="B16" s="45">
-        <f>Касса!A40</f>
+        <f>Касса!A39</f>
         <v>0</v>
       </c>
       <c r="C16" s="46">
-        <f>Касса!C40</f>
+        <f>Касса!C39</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
-        <f>Касса!B41</f>
+        <f>Касса!B40</f>
         <v>0</v>
       </c>
       <c r="B17" s="45">
-        <f>Касса!A41</f>
+        <f>Касса!A40</f>
         <v>0</v>
       </c>
       <c r="C17" s="46">
-        <f>Касса!C41</f>
+        <f>Касса!C40</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
+        <f>Касса!B41</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="45">
+        <f>Касса!A41</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="46">
+        <f>Касса!C41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
         <f>Касса!B42</f>
         <v>0</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B19" s="45">
         <f>Касса!A42</f>
         <v>0</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C19" s="46">
         <f>Касса!C42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="43" t="s">
+    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="47"/>
-    </row>
-    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
-        <f>Касса!E7</f>
-        <v>0</v>
-      </c>
-      <c r="B20" s="45">
-        <f>Касса!D7</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="46">
-        <f>Касса!F7</f>
-        <v>0</v>
-      </c>
+      <c r="C20" s="47"/>
     </row>
     <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
-        <f>Касса!E8</f>
+        <f>Касса!E7</f>
         <v>0</v>
       </c>
       <c r="B21" s="45">
-        <f>Касса!D8</f>
+        <f>Касса!D7</f>
         <v>0</v>
       </c>
       <c r="C21" s="46">
-        <f>Касса!F8</f>
+        <f>Касса!F7</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
-        <f>Касса!E9</f>
+        <f>Касса!E8</f>
         <v>0</v>
       </c>
       <c r="B22" s="45">
-        <f>Касса!D9</f>
+        <f>Касса!D8</f>
         <v>0</v>
       </c>
       <c r="C22" s="46">
-        <f>Касса!F9</f>
+        <f>Касса!F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
+        <f>Касса!E9</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="45">
+        <f>Касса!D9</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="46">
+        <f>Касса!F9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
         <f>Касса!E10</f>
         <v>0</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B24" s="45">
         <f>Касса!D10</f>
         <v>0</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C24" s="46">
         <f>Касса!F10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="48"/>
-      <c r="B24" s="43" t="s">
+    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="48"/>
+      <c r="B25" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="49"/>
-    </row>
-    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
-        <f>Касса!E12</f>
-        <v>0</v>
-      </c>
-      <c r="B25" s="45">
-        <f>Касса!D12</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="46">
-        <f>Касса!F12</f>
-        <v>0</v>
-      </c>
+      <c r="C25" s="49"/>
     </row>
     <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
-        <f>Касса!E13</f>
+        <f>Касса!E12</f>
         <v>0</v>
       </c>
       <c r="B26" s="45">
-        <f>Касса!D13</f>
+        <f>Касса!D12</f>
         <v>0</v>
       </c>
       <c r="C26" s="46">
-        <f>Касса!F13</f>
+        <f>Касса!F12</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
-        <f>Касса!E14</f>
+        <f>Касса!E13</f>
         <v>0</v>
       </c>
       <c r="B27" s="45">
-        <f>Касса!D14</f>
+        <f>Касса!D13</f>
         <v>0</v>
       </c>
       <c r="C27" s="46">
-        <f>Касса!F14</f>
+        <f>Касса!F13</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
-        <f>Касса!E15</f>
+        <f>Касса!E14</f>
         <v>0</v>
       </c>
       <c r="B28" s="45">
-        <f>Касса!D15</f>
+        <f>Касса!D14</f>
         <v>0</v>
       </c>
       <c r="C28" s="46">
-        <f>Касса!F15</f>
+        <f>Касса!F14</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
-        <f>Касса!E16</f>
+        <f>Касса!E15</f>
         <v>0</v>
       </c>
       <c r="B29" s="45">
-        <f>Касса!D16</f>
+        <f>Касса!D15</f>
         <v>0</v>
       </c>
       <c r="C29" s="46">
-        <f>Касса!F16</f>
+        <f>Касса!F15</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
+        <f>Касса!E16</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="45">
+        <f>Касса!D16</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="46">
+        <f>Касса!F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="38">
         <f>Касса!E17</f>
         <v>0</v>
       </c>
-      <c r="B30" s="45">
+      <c r="B31" s="45">
         <f>Касса!D17</f>
         <v>0</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C31" s="46">
         <f>Касса!F17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="43" t="s">
+    <row r="32" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38"/>
+      <c r="B32" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="50"/>
-    </row>
-    <row r="32" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38">
-        <f>Касса!E19</f>
-        <v>0</v>
-      </c>
-      <c r="B32" s="45">
-        <f>Касса!D19</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="46">
-        <f>Касса!F19</f>
-        <v>0</v>
-      </c>
+      <c r="C32" s="50"/>
     </row>
     <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
-        <f>Касса!E20</f>
+        <f>Касса!E19</f>
         <v>0</v>
       </c>
       <c r="B33" s="45">
-        <f>Касса!D20</f>
+        <f>Касса!D19</f>
         <v>0</v>
       </c>
       <c r="C33" s="46">
-        <f>Касса!F20</f>
+        <f>Касса!F19</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
-        <f>Касса!E21</f>
+        <f>Касса!E20</f>
         <v>0</v>
       </c>
       <c r="B34" s="45">
-        <f>Касса!D21</f>
+        <f>Касса!D20</f>
         <v>0</v>
       </c>
       <c r="C34" s="46">
-        <f>Касса!F21</f>
+        <f>Касса!F20</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
-        <f>Касса!E22</f>
+        <f>Касса!E21</f>
         <v>0</v>
       </c>
       <c r="B35" s="45">
-        <f>Касса!D22</f>
+        <f>Касса!D21</f>
         <v>0</v>
       </c>
       <c r="C35" s="46">
-        <f>Касса!F22</f>
+        <f>Касса!F21</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
-        <f>Касса!E23</f>
+        <f>Касса!E22</f>
         <v>0</v>
       </c>
       <c r="B36" s="45">
-        <f>Касса!D23</f>
+        <f>Касса!D22</f>
         <v>0</v>
       </c>
       <c r="C36" s="46">
-        <f>Касса!F23</f>
+        <f>Касса!F22</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
+        <f>Касса!E23</f>
+        <v>0</v>
+      </c>
+      <c r="B37" s="45">
+        <f>Касса!D23</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="46">
+        <f>Касса!F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
         <f>Касса!E24</f>
         <v>0</v>
       </c>
-      <c r="B37" s="45">
+      <c r="B38" s="45">
         <f>Касса!D24</f>
         <v>0</v>
       </c>
-      <c r="C37" s="46">
+      <c r="C38" s="46">
         <f>Касса!F24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="B38" s="43" t="s">
+    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="38"/>
+      <c r="B39" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="49"/>
-    </row>
-    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38">
-        <f>Касса!E26</f>
-        <v>0</v>
-      </c>
-      <c r="B39" s="45">
-        <f>Касса!D26</f>
-        <v>0</v>
-      </c>
-      <c r="C39" s="46">
-        <f>Касса!F26</f>
-        <v>0</v>
-      </c>
+      <c r="C39" s="49"/>
     </row>
     <row r="40" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="38">
-        <f>Касса!E27</f>
+        <f>Касса!E26</f>
         <v>0</v>
       </c>
       <c r="B40" s="45">
-        <f>Касса!D27</f>
+        <f>Касса!D26</f>
         <v>0</v>
       </c>
       <c r="C40" s="46">
-        <f>Касса!F27</f>
+        <f>Касса!F26</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="38">
-        <f>Касса!E28</f>
+        <f>Касса!E27</f>
         <v>0</v>
       </c>
       <c r="B41" s="45">
-        <f>Касса!D28</f>
+        <f>Касса!D27</f>
         <v>0</v>
       </c>
       <c r="C41" s="46">
-        <f>Касса!F28</f>
+        <f>Касса!F27</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
+        <f>Касса!E28</f>
+        <v>0</v>
+      </c>
+      <c r="B42" s="45">
+        <f>Касса!D28</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="46">
+        <f>Касса!F28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="38">
         <f>Касса!E29</f>
         <v>0</v>
       </c>
-      <c r="B42" s="45">
+      <c r="B43" s="45">
         <f>Касса!D29</f>
         <v>0</v>
       </c>
-      <c r="C42" s="46">
+      <c r="C43" s="46">
         <f>Касса!F29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="51"/>
-      <c r="B43" s="43" t="s">
+    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="51"/>
+      <c r="B44" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="50"/>
-    </row>
-    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38">
-        <f>Касса!E31</f>
-        <v>0</v>
-      </c>
-      <c r="B44" s="45">
-        <f>Касса!D31</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="46">
-        <f>Касса!F31</f>
-        <v>0</v>
-      </c>
+      <c r="C44" s="50"/>
     </row>
     <row r="45" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="38">
-        <f>Касса!E32</f>
+        <f>Касса!E31</f>
         <v>0</v>
       </c>
       <c r="B45" s="45">
-        <f>Касса!D32</f>
+        <f>Касса!D31</f>
         <v>0</v>
       </c>
       <c r="C45" s="46">
-        <f>Касса!F32</f>
+        <f>Касса!F31</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="38">
-        <f>Касса!E33</f>
+        <f>Касса!E32</f>
         <v>0</v>
       </c>
       <c r="B46" s="45">
-        <f>Касса!D33</f>
+        <f>Касса!D32</f>
         <v>0</v>
       </c>
       <c r="C46" s="46">
-        <f>Касса!F33</f>
+        <f>Касса!F32</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="38">
-        <f>Касса!E34</f>
+        <f>Касса!E33</f>
         <v>0</v>
       </c>
       <c r="B47" s="45">
-        <f>Касса!D34</f>
+        <f>Касса!D33</f>
         <v>0</v>
       </c>
       <c r="C47" s="46">
-        <f>Касса!F34</f>
+        <f>Касса!F33</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="38">
-        <f>Касса!E35</f>
+        <f>Касса!E34</f>
         <v>0</v>
       </c>
       <c r="B48" s="45">
-        <f>Касса!D35</f>
+        <f>Касса!D34</f>
         <v>0</v>
       </c>
       <c r="C48" s="46">
-        <f>Касса!F35</f>
+        <f>Касса!F34</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
-        <f>Касса!E36</f>
+        <f>Касса!E35</f>
         <v>0</v>
       </c>
       <c r="B49" s="45">
-        <f>Касса!D36</f>
+        <f>Касса!D35</f>
         <v>0</v>
       </c>
       <c r="C49" s="46">
-        <f>Касса!F36</f>
+        <f>Касса!F35</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="38">
-        <f>Касса!E37</f>
+        <f>Касса!E36</f>
         <v>0</v>
       </c>
       <c r="B50" s="45">
-        <f>Касса!D37</f>
+        <f>Касса!D36</f>
         <v>0</v>
       </c>
       <c r="C50" s="46">
-        <f>Касса!F37</f>
+        <f>Касса!F36</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="38">
+        <f>Касса!E37</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="45">
+        <f>Касса!D37</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="46">
+        <f>Касса!F37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="38">
         <f>Касса!E38</f>
         <v>0</v>
       </c>
-      <c r="B51" s="45">
+      <c r="B52" s="45">
         <f>Касса!D38</f>
         <v>0</v>
       </c>
-      <c r="C51" s="46">
+      <c r="C52" s="46">
         <f>Касса!F38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="48"/>
-      <c r="B52" s="43" t="s">
+    <row r="53" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="48"/>
+      <c r="B53" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="50"/>
-    </row>
-    <row r="53" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="C53" s="50"/>
     </row>
     <row r="54" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="46">
-        <v>75</v>
+      <c r="A54" s="38" t="str">
+        <f>Касса!E40</f>
+        <v>200/300мл</v>
+      </c>
+      <c r="B54" s="45" t="str">
+        <f>Касса!D40</f>
+        <v>Напиток охл.в стакане/в бутылке</v>
+      </c>
+      <c r="C54" s="46" t="str">
+        <f>Касса!F40</f>
+        <v>60/80</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="82" t="str">
+      <c r="A55" s="38" t="str">
+        <f>Касса!E43</f>
+        <v>225мл</v>
+      </c>
+      <c r="B55" s="45" t="str">
+        <f>Касса!D43</f>
+        <v>Чай фруктовый в ассортименте</v>
+      </c>
+      <c r="C55" s="46">
+        <f>Касса!F43</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="81" t="str">
         <f>Касса!A60</f>
         <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
       </c>
-      <c r="B55" s="78"/>
-      <c r="C55" s="78"/>
-    </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="83" t="str">
+      <c r="B56" s="77"/>
+      <c r="C56" s="77"/>
+    </row>
+    <row r="57" spans="1:3" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="82" t="str">
         <f>Касса!A61</f>
         <v>Блюда могут содержать следы молочных продуктов, яичных продуктов, рыбы, моллюсков, кунжута, горчицы, сои, злаков, содержащих глютен, арахиса, аспартама, диоксида серы и сульфатов, люпина, орехов, ракообразных, сельдерея. Допускается использовать аналогичные указанным компоненты, отечественного или импортного производства, соответствующие нормативным и правовым документам Российской Федерации и Таможенного союза.</v>
       </c>
-      <c r="B56" s="78"/>
-      <c r="C56" s="78"/>
-    </row>
-    <row r="57" spans="1:3" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="78"/>
-      <c r="B57" s="78"/>
-      <c r="C57" s="78"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="77"/>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="78"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="78"/>
+      <c r="A58" s="77"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="77"/>
+    </row>
+    <row r="59" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="77"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A56:C58"/>
-    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A57:C59"/>
+    <mergeCell ref="A56:C56"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0" bottom="0" header="0.11811023622047249" footer="0.11811023622047249"/>
   <pageSetup paperSize="9" scale="70" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3822,8 +3844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3851,32 +3873,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="79" t="str">
+      <c r="B2" s="78" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
+      <c r="E2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="80" t="str">
+      <c r="B3" s="79" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -3894,22 +3916,22 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="20"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -3927,7 +3949,7 @@
       <c r="K6" s="20"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <f>Касса!A7</f>
         <v>0</v>
@@ -3947,7 +3969,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <f>Касса!A8</f>
         <v>0</v>
@@ -3967,7 +3989,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <f>Касса!A9</f>
         <v>0</v>
@@ -3987,7 +4009,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <f>Касса!A10</f>
         <v>0</v>
@@ -4007,7 +4029,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f>Касса!A11</f>
         <v>0</v>
@@ -4026,7 +4048,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f>Касса!A12</f>
         <v>0</v>
@@ -4046,7 +4068,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <f>Касса!A13</f>
         <v>0</v>
@@ -4066,7 +4088,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <f>Касса!A14</f>
         <v>0</v>
@@ -4086,7 +4108,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <f>Касса!A15</f>
         <v>0</v>
@@ -4106,7 +4128,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <f>Касса!A16</f>
         <v>0</v>
@@ -4126,7 +4148,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <f>Касса!A17</f>
         <v>0</v>
@@ -4146,7 +4168,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <f>Касса!A18</f>
         <v>0</v>
@@ -4165,7 +4187,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <f>Касса!A19</f>
         <v>0</v>
@@ -4185,7 +4207,7 @@
       <c r="K19" s="20"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <f>Касса!A20</f>
         <v>0</v>
@@ -4205,7 +4227,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="18"/>
     </row>
-    <row r="21" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <f>Касса!A21</f>
         <v>0</v>
@@ -4225,7 +4247,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <f>Касса!A22</f>
         <v>0</v>
@@ -4245,7 +4267,7 @@
       <c r="K22" s="20"/>
       <c r="L22" s="18"/>
     </row>
-    <row r="23" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <f>Касса!A23</f>
         <v>0</v>
@@ -4265,7 +4287,7 @@
       <c r="K23" s="20"/>
       <c r="L23" s="18"/>
     </row>
-    <row r="24" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <f>Касса!A24</f>
         <v>0</v>
@@ -4285,7 +4307,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="18"/>
     </row>
-    <row r="25" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <f>Касса!A25</f>
         <v>0</v>
@@ -4304,7 +4326,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="18"/>
     </row>
-    <row r="26" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <f>Касса!A26</f>
         <v>0</v>
@@ -4324,7 +4346,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="18"/>
     </row>
-    <row r="27" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <f>Касса!A27</f>
         <v>0</v>
@@ -4344,7 +4366,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="18"/>
     </row>
-    <row r="28" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <f>Касса!A28</f>
         <v>0</v>
@@ -4364,11 +4386,8 @@
       <c r="K28" s="20"/>
       <c r="L28" s="18"/>
     </row>
-    <row r="29" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <f>Касса!A29</f>
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="11"/>
@@ -4384,7 +4403,7 @@
       <c r="K29" s="20"/>
       <c r="L29" s="18"/>
     </row>
-    <row r="30" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="52"/>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -4400,7 +4419,7 @@
       <c r="K30" s="20"/>
       <c r="L30" s="18"/>
     </row>
-    <row r="31" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10"/>
       <c r="B31" s="15"/>
       <c r="C31" s="54"/>
@@ -4417,7 +4436,7 @@
       <c r="K31" s="20"/>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="15"/>
       <c r="C32" s="54"/>
@@ -4434,7 +4453,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="18"/>
     </row>
-    <row r="33" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10"/>
       <c r="B33" s="15"/>
       <c r="C33" s="54"/>
@@ -4451,7 +4470,7 @@
       <c r="K33" s="20"/>
       <c r="L33" s="18"/>
     </row>
-    <row r="34" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10"/>
       <c r="B34" s="15"/>
       <c r="C34" s="54"/>
@@ -4468,7 +4487,7 @@
       <c r="K34" s="20"/>
       <c r="L34" s="18"/>
     </row>
-    <row r="35" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10"/>
       <c r="B35" s="15"/>
       <c r="C35" s="54"/>
@@ -4485,7 +4504,7 @@
       <c r="K35" s="20"/>
       <c r="L35" s="18"/>
     </row>
-    <row r="36" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="15"/>
       <c r="C36" s="54"/>
@@ -4502,7 +4521,7 @@
       <c r="K36" s="20"/>
       <c r="L36" s="18"/>
     </row>
-    <row r="37" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10"/>
       <c r="B37" s="15"/>
       <c r="C37" s="54"/>
@@ -4519,7 +4538,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="18"/>
     </row>
-    <row r="38" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10"/>
       <c r="B38" s="15"/>
       <c r="C38" s="54"/>
@@ -4536,7 +4555,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="18"/>
     </row>
-    <row r="39" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
       <c r="B39" s="15"/>
       <c r="C39" s="54"/>
@@ -4551,13 +4570,13 @@
       <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="85"/>
-      <c r="B40" s="78"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
+      <c r="A40" s="84"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
       <c r="H40" s="57"/>
       <c r="I40" s="58"/>
       <c r="J40" s="18"/>
@@ -4565,13 +4584,13 @@
       <c r="L40" s="18"/>
     </row>
     <row r="41" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="76"/>
-      <c r="B41" s="78"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
+      <c r="A41" s="75"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
       <c r="H41" s="59"/>
       <c r="I41" s="58"/>
       <c r="J41" s="18"/>
@@ -4791,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4820,32 +4839,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="79" t="str">
+      <c r="B2" s="78" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
+      <c r="E2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="80" t="str">
+      <c r="B3" s="79" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -4863,15 +4882,15 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -4883,10 +4902,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="52"/>
       <c r="E6" s="52"/>
@@ -4900,11 +4919,11 @@
     </row>
     <row r="7" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
-        <f>Касса!A31</f>
+        <f>Касса!A30</f>
         <v>0</v>
       </c>
       <c r="B7" s="3">
-        <f>Касса!B31</f>
+        <f>Касса!B30</f>
         <v>0</v>
       </c>
       <c r="C7" s="15"/>
@@ -4920,11 +4939,11 @@
     </row>
     <row r="8" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <f>Касса!A32</f>
+        <f>Касса!A31</f>
         <v>0</v>
       </c>
       <c r="B8" s="3">
-        <f>Касса!B32</f>
+        <f>Касса!B31</f>
         <v>0</v>
       </c>
       <c r="C8" s="15"/>
@@ -4940,11 +4959,11 @@
     </row>
     <row r="9" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
-        <f>Касса!A33</f>
+        <f>Касса!A32</f>
         <v>0</v>
       </c>
       <c r="B9" s="3">
-        <f>Касса!B33</f>
+        <f>Касса!B32</f>
         <v>0</v>
       </c>
       <c r="C9" s="15"/>
@@ -4960,11 +4979,11 @@
     </row>
     <row r="10" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <f>Касса!A34</f>
+        <f>Касса!A33</f>
         <v>0</v>
       </c>
       <c r="B10" s="3">
-        <f>Касса!B34</f>
+        <f>Касса!B33</f>
         <v>0</v>
       </c>
       <c r="C10" s="15"/>
@@ -4980,11 +4999,11 @@
     </row>
     <row r="11" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
-        <f>Касса!A35</f>
+        <f>Касса!A34</f>
         <v>0</v>
       </c>
       <c r="B11" s="3">
-        <f>Касса!B35</f>
+        <f>Касса!B34</f>
         <v>0</v>
       </c>
       <c r="C11" s="15"/>
@@ -5000,11 +5019,11 @@
     </row>
     <row r="12" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <f>Касса!A36</f>
+        <f>Касса!A35</f>
         <v>0</v>
       </c>
       <c r="B12" s="3">
-        <f>Касса!B36</f>
+        <f>Касса!B35</f>
         <v>0</v>
       </c>
       <c r="C12" s="15"/>
@@ -5020,11 +5039,11 @@
     </row>
     <row r="13" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
-        <f>Касса!A37</f>
+        <f>Касса!A36</f>
         <v>0</v>
       </c>
       <c r="B13" s="3">
-        <f>Касса!B37</f>
+        <f>Касса!B36</f>
         <v>0</v>
       </c>
       <c r="C13" s="15"/>
@@ -5040,14 +5059,14 @@
     </row>
     <row r="14" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <f>Касса!A38</f>
+        <f>Касса!A37</f>
         <v>0</v>
       </c>
       <c r="B14" s="3">
-        <f>Касса!B38</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="64"/>
+        <f>Касса!B37</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="53"/>
       <c r="E14" s="23"/>
       <c r="F14" s="15"/>
@@ -5060,14 +5079,14 @@
     </row>
     <row r="15" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
-        <f>Касса!A39</f>
+        <f>Касса!A38</f>
         <v>0</v>
       </c>
       <c r="B15" s="3">
-        <f>Касса!B39</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="15"/>
+        <f>Касса!B38</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="63"/>
       <c r="D15" s="53"/>
       <c r="E15" s="10"/>
       <c r="F15" s="15"/>
@@ -5080,14 +5099,14 @@
     </row>
     <row r="16" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
-        <f>Касса!A40</f>
+        <f>Касса!A39</f>
         <v>0</v>
       </c>
       <c r="B16" s="3">
-        <f>Касса!B40</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="64"/>
+        <f>Касса!B39</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="15"/>
       <c r="D16" s="53"/>
       <c r="E16" s="10"/>
       <c r="F16" s="15"/>
@@ -5100,14 +5119,14 @@
     </row>
     <row r="17" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <f>Касса!A41</f>
+        <f>Касса!A40</f>
         <v>0</v>
       </c>
       <c r="B17" s="3">
-        <f>Касса!B41</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="15"/>
+        <f>Касса!B40</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="63"/>
       <c r="D17" s="53"/>
       <c r="E17" s="10"/>
       <c r="F17" s="15"/>
@@ -5119,13 +5138,13 @@
       <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="e">
-        <f>LEFT(Касса!A42,FIND("/",Касса!A42)-1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B18" s="3" t="e">
-        <f>LEFT(Касса!B42,FIND("/",Касса!B42)-1) &amp; "г"</f>
-        <v>#VALUE!</v>
+      <c r="A18" s="6">
+        <f>Касса!A41</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="3">
+        <f>Касса!B41</f>
+        <v>0</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="53"/>
@@ -5140,15 +5159,15 @@
     </row>
     <row r="19" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="e">
-        <f>"Цезарь "&amp;MID(Касса!A42,FIND("/",Касса!A42)+1,999)</f>
+        <f>LEFT(Касса!A42,FIND("/",Касса!A42)-1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="B19" s="3" t="e">
-        <f>MID(Касса!B42,FIND("/",Касса!B42)+1,999)</f>
+        <f>LEFT(Касса!B42,FIND("/",Касса!B42)-1) &amp; "г"</f>
         <v>#VALUE!</v>
       </c>
       <c r="C19" s="15"/>
-      <c r="D19" s="65"/>
+      <c r="D19" s="64"/>
       <c r="E19" s="10"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -5159,14 +5178,15 @@
       <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53">
-        <f>SUM(C7:C19)</f>
-        <v>0</v>
-      </c>
+      <c r="A20" s="10" t="e">
+        <f>"Цезарь "&amp;MID(Касса!A42,FIND("/",Касса!A42)+1,999)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B20" s="3" t="e">
+        <f>MID(Касса!B42,FIND("/",Касса!B42)+1,999)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="15"/>
       <c r="D20" s="53"/>
       <c r="E20" s="10"/>
       <c r="F20" s="15"/>
@@ -5178,9 +5198,14 @@
       <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53">
+        <f>SUM(C8:C20)</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="53"/>
       <c r="E21" s="10"/>
       <c r="F21" s="15"/>
@@ -5192,9 +5217,7 @@
       <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="A22" s="6"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="53"/>
@@ -5208,14 +5231,10 @@
       <c r="L22" s="18"/>
     </row>
     <row r="23" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="str">
-        <f>Касса!A44</f>
-        <v>Сэндвич с бужениной</v>
-      </c>
-      <c r="B23" s="3" t="str">
-        <f>Касса!B44</f>
-        <v>180г</v>
-      </c>
+      <c r="A23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="53"/>
       <c r="E23" s="10"/>
@@ -5229,11 +5248,11 @@
     </row>
     <row r="24" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="str">
-        <f>Касса!A45</f>
-        <v>Сэндвич с ветчиной и сыром</v>
+        <f>Касса!A44</f>
+        <v>Сэндвич с бужениной</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f>Касса!B45</f>
+        <f>Касса!B44</f>
         <v>180г</v>
       </c>
       <c r="C24" s="15"/>
@@ -5249,11 +5268,11 @@
     </row>
     <row r="25" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="str">
-        <f>Касса!A46</f>
-        <v>Сэндвич с куриной грудкой</v>
+        <f>Касса!A45</f>
+        <v>Сэндвич с ветчиной и сыром</v>
       </c>
       <c r="B25" s="3" t="str">
-        <f>Касса!B46</f>
+        <f>Касса!B45</f>
         <v>180г</v>
       </c>
       <c r="C25" s="15"/>
@@ -5269,15 +5288,15 @@
     </row>
     <row r="26" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="str">
-        <f>Касса!A47</f>
-        <v>Сэндвич с форелью</v>
+        <f>Касса!A46</f>
+        <v>Сэндвич с куриной грудкой</v>
       </c>
       <c r="B26" s="3" t="str">
-        <f>Касса!B47</f>
+        <f>Касса!B46</f>
         <v>180г</v>
       </c>
       <c r="C26" s="15"/>
-      <c r="D26" s="53"/>
+      <c r="D26" s="86"/>
       <c r="E26" s="23"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -5288,13 +5307,19 @@
       <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="63"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="6" t="str">
+        <f>Касса!A47</f>
+        <v>Сэндвич с форелью</v>
+      </c>
+      <c r="B27" s="3" t="str">
+        <f>Касса!B47</f>
+        <v>180г</v>
+      </c>
       <c r="C27" s="15"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="54"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="H27" s="19"/>
       <c r="I27" s="20"/>
       <c r="J27" s="18"/>
@@ -5305,10 +5330,6 @@
       <c r="A28" s="30"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
       <c r="H28" s="19"/>
       <c r="I28" s="20"/>
       <c r="J28" s="18"/>
@@ -5599,8 +5620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5628,32 +5649,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="79" t="str">
+      <c r="B2" s="78" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
+      <c r="E2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="80" t="str">
+      <c r="B3" s="79" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -5671,40 +5692,40 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="20"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="19"/>
@@ -5712,7 +5733,7 @@
       <c r="K6" s="20"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <f>Касса!A7</f>
         <v>0</v>
@@ -5732,7 +5753,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <f>Касса!A8</f>
         <v>0</v>
@@ -5752,7 +5773,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <f>Касса!A9</f>
         <v>0</v>
@@ -5772,7 +5793,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <f>Касса!A10</f>
         <v>0</v>
@@ -5792,7 +5813,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f>Касса!A11</f>
         <v>0</v>
@@ -5811,7 +5832,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f>Касса!A12</f>
         <v>0</v>
@@ -5831,7 +5852,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <f>Касса!A13</f>
         <v>0</v>
@@ -5851,7 +5872,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <f>Касса!A14</f>
         <v>0</v>
@@ -5871,7 +5892,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <f>Касса!A15</f>
         <v>0</v>
@@ -5891,7 +5912,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <f>Касса!A16</f>
         <v>0</v>
@@ -5911,7 +5932,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <f>Касса!A17</f>
         <v>0</v>
@@ -5931,7 +5952,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <f>Касса!A18</f>
         <v>0</v>
@@ -5950,7 +5971,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <f>Касса!A19</f>
         <v>0</v>
@@ -5970,7 +5991,7 @@
       <c r="K19" s="20"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <f>Касса!A20</f>
         <v>0</v>
@@ -5990,7 +6011,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="18"/>
     </row>
-    <row r="21" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <f>Касса!A21</f>
         <v>0</v>
@@ -6010,7 +6031,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <f>Касса!A22</f>
         <v>0</v>
@@ -6030,7 +6051,7 @@
       <c r="K22" s="20"/>
       <c r="L22" s="18"/>
     </row>
-    <row r="23" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <f>Касса!A23</f>
         <v>0</v>
@@ -6050,7 +6071,7 @@
       <c r="K23" s="20"/>
       <c r="L23" s="18"/>
     </row>
-    <row r="24" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <f>Касса!A24</f>
         <v>0</v>
@@ -6070,7 +6091,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="18"/>
     </row>
-    <row r="25" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <f>Касса!A25</f>
         <v>0</v>
@@ -6089,7 +6110,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="18"/>
     </row>
-    <row r="26" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <f>Касса!A26</f>
         <v>0</v>
@@ -6109,7 +6130,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="18"/>
     </row>
-    <row r="27" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <f>Касса!A27</f>
         <v>0</v>
@@ -6129,7 +6150,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="18"/>
     </row>
-    <row r="28" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <f>Касса!A28</f>
         <v>0</v>
@@ -6149,10 +6170,9 @@
       <c r="K28" s="20"/>
       <c r="L28" s="18"/>
     </row>
-    <row r="29" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <f>Касса!A29</f>
-        <v>0</v>
+    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6169,9 +6189,10 @@
       <c r="K29" s="20"/>
       <c r="L29" s="18"/>
     </row>
-    <row r="30" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
-        <v>14</v>
+    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
+        <f>Касса!A30</f>
+        <v>0</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -6187,7 +6208,7 @@
       <c r="K30" s="20"/>
       <c r="L30" s="18"/>
     </row>
-    <row r="31" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <f>Касса!A31</f>
         <v>0</v>
@@ -6207,7 +6228,7 @@
       <c r="K31" s="20"/>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <f>Касса!A32</f>
         <v>0</v>
@@ -6227,7 +6248,7 @@
       <c r="K32" s="20"/>
       <c r="L32" s="18"/>
     </row>
-    <row r="33" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <f>Касса!A33</f>
         <v>0</v>
@@ -6247,7 +6268,7 @@
       <c r="K33" s="20"/>
       <c r="L33" s="18"/>
     </row>
-    <row r="34" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <f>Касса!A34</f>
         <v>0</v>
@@ -6267,7 +6288,7 @@
       <c r="K34" s="20"/>
       <c r="L34" s="18"/>
     </row>
-    <row r="35" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <f>Касса!A35</f>
         <v>0</v>
@@ -6287,7 +6308,7 @@
       <c r="K35" s="20"/>
       <c r="L35" s="18"/>
     </row>
-    <row r="36" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <f>Касса!A36</f>
         <v>0</v>
@@ -6307,7 +6328,7 @@
       <c r="K36" s="20"/>
       <c r="L36" s="18"/>
     </row>
-    <row r="37" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <f>Касса!A37</f>
         <v>0</v>
@@ -6327,7 +6348,7 @@
       <c r="K37" s="20"/>
       <c r="L37" s="18"/>
     </row>
-    <row r="38" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <f>Касса!A38</f>
         <v>0</v>
@@ -6347,7 +6368,7 @@
       <c r="K38" s="20"/>
       <c r="L38" s="18"/>
     </row>
-    <row r="39" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <f>Касса!A39</f>
         <v>0</v>
@@ -6360,11 +6381,11 @@
       <c r="G39" s="53"/>
       <c r="H39" s="57"/>
       <c r="I39" s="58"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="67"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="66"/>
       <c r="L39" s="18"/>
     </row>
-    <row r="40" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <f>Касса!A40</f>
         <v>0</v>
@@ -6377,11 +6398,11 @@
       <c r="G40" s="15"/>
       <c r="H40" s="57"/>
       <c r="I40" s="58"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="67"/>
+      <c r="J40" s="65"/>
+      <c r="K40" s="66"/>
       <c r="L40" s="18"/>
     </row>
-    <row r="41" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <f>Касса!A41</f>
         <v>0</v>
@@ -6394,11 +6415,11 @@
       <c r="G41" s="54"/>
       <c r="H41" s="59"/>
       <c r="I41" s="58"/>
-      <c r="J41" s="66"/>
-      <c r="K41" s="67"/>
+      <c r="J41" s="65"/>
+      <c r="K41" s="66"/>
       <c r="L41" s="18"/>
     </row>
-    <row r="42" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <f>Касса!A42</f>
         <v>0</v>
@@ -6411,50 +6432,50 @@
       <c r="G42" s="54"/>
       <c r="H42" s="57"/>
       <c r="I42" s="58"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="67"/>
+      <c r="J42" s="65"/>
+      <c r="K42" s="66"/>
       <c r="L42" s="18"/>
     </row>
-    <row r="43" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="53"/>
       <c r="B43" s="55"/>
       <c r="C43" s="56"/>
-      <c r="D43" s="65"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="10"/>
       <c r="F43" s="15"/>
       <c r="G43" s="54"/>
       <c r="H43" s="60"/>
       <c r="I43" s="58"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="67"/>
+      <c r="J43" s="65"/>
+      <c r="K43" s="66"/>
       <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="86"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
       <c r="H44" s="61"/>
       <c r="I44" s="58"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="67"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="66"/>
       <c r="L44" s="18"/>
     </row>
     <row r="45" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="76"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
+      <c r="A45" s="75"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
       <c r="H45" s="59"/>
       <c r="I45" s="58"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="67"/>
+      <c r="J45" s="65"/>
+      <c r="K45" s="66"/>
       <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6467,8 +6488,8 @@
       <c r="G46" s="30"/>
       <c r="H46" s="59"/>
       <c r="I46" s="58"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="67"/>
+      <c r="J46" s="65"/>
+      <c r="K46" s="66"/>
       <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6481,8 +6502,8 @@
       <c r="G47" s="28"/>
       <c r="H47" s="59"/>
       <c r="I47" s="58"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="67"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="66"/>
       <c r="L47" s="18"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6495,64 +6516,64 @@
       <c r="G48" s="28"/>
       <c r="H48" s="59"/>
       <c r="I48" s="58"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="67"/>
+      <c r="J48" s="65"/>
+      <c r="K48" s="66"/>
       <c r="L48" s="18"/>
     </row>
     <row r="49" spans="8:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H49" s="61"/>
       <c r="I49" s="58"/>
-      <c r="J49" s="66"/>
-      <c r="K49" s="67"/>
+      <c r="J49" s="65"/>
+      <c r="K49" s="66"/>
       <c r="L49" s="18"/>
     </row>
     <row r="50" spans="8:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H50" s="59"/>
       <c r="I50" s="58"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="67"/>
+      <c r="J50" s="65"/>
+      <c r="K50" s="66"/>
       <c r="L50" s="18"/>
     </row>
     <row r="51" spans="8:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H51" s="59"/>
       <c r="I51" s="58"/>
-      <c r="J51" s="66"/>
-      <c r="K51" s="67"/>
+      <c r="J51" s="65"/>
+      <c r="K51" s="66"/>
       <c r="L51" s="18"/>
     </row>
     <row r="52" spans="8:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H52" s="59"/>
       <c r="I52" s="58"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="67"/>
+      <c r="J52" s="65"/>
+      <c r="K52" s="66"/>
       <c r="L52" s="18"/>
     </row>
     <row r="53" spans="8:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H53" s="59"/>
       <c r="I53" s="58"/>
-      <c r="J53" s="66"/>
-      <c r="K53" s="67"/>
+      <c r="J53" s="65"/>
+      <c r="K53" s="66"/>
       <c r="L53" s="18"/>
     </row>
     <row r="54" spans="8:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H54" s="59"/>
       <c r="I54" s="58"/>
-      <c r="J54" s="66"/>
-      <c r="K54" s="66"/>
+      <c r="J54" s="65"/>
+      <c r="K54" s="65"/>
       <c r="L54" s="18"/>
     </row>
     <row r="55" spans="8:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H55" s="59"/>
       <c r="I55" s="58"/>
-      <c r="J55" s="66"/>
-      <c r="K55" s="66"/>
+      <c r="J55" s="65"/>
+      <c r="K55" s="65"/>
       <c r="L55" s="18"/>
     </row>
     <row r="56" spans="8:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H56" s="59"/>
       <c r="I56" s="58"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="66"/>
+      <c r="J56" s="65"/>
+      <c r="K56" s="65"/>
       <c r="L56" s="18"/>
     </row>
     <row r="57" spans="8:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update menu template and add icon files
</commit_message>
<xml_diff>
--- a/excel_menu_gui/templates/Шаблон меню пример.xlsx
+++ b/excel_menu_gui/templates/Шаблон меню пример.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katya\Desktop\menurepit\excel_menu_gui\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98845E1-521D-4447-A797-DB18AA0B120C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5BD0E7-D830-4E7C-B05B-6B68AB2A7314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="447" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Касса" sheetId="1" r:id="rId1"/>
     <sheet name="Завтрак" sheetId="2" r:id="rId2"/>
-    <sheet name="Гц" sheetId="4" r:id="rId3"/>
-    <sheet name="Обед" sheetId="3" r:id="rId4"/>
+    <sheet name="Обед" sheetId="3" r:id="rId3"/>
+    <sheet name="Гц" sheetId="4" r:id="rId4"/>
     <sheet name="Хц" sheetId="5" r:id="rId5"/>
     <sheet name="Раздача" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Завтрак!$A$1:$C$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Обед!$A$1:$G$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Обед!$A$1:$G$66</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Раздача!$A$1:$G$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Хц!$A$1:$G$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Хц!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t xml:space="preserve">Утверждаю </t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>225мл</t>
+  </si>
+  <si>
+    <t>4 и 4</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -794,6 +797,7 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -824,10 +828,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -963,6 +963,61 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24602" name="Рисунок 1" descr="Логотип-(Патриот)">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001A600000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="76200" y="152400"/>
+          <a:ext cx="2038350" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -997,61 +1052,6 @@
         <a:xfrm>
           <a:off x="133350" y="95250"/>
           <a:ext cx="1854200" cy="596900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24602" name="Рисунок 1" descr="Логотип-(Патриот)">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001A600000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="76200" y="152400"/>
-          <a:ext cx="2038350" cy="895350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1536,7 +1536,7 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1562,28 +1562,28 @@
     </row>
     <row r="2" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="73" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -1600,14 +1600,14 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="1"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -2530,14 +2530,14 @@
       <c r="K58" s="18"/>
     </row>
     <row r="59" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="78" t="s">
+      <c r="A59" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="78"/>
-      <c r="C59" s="78"/>
-      <c r="D59" s="78"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="79"/>
+      <c r="F59" s="79"/>
       <c r="G59" s="1"/>
       <c r="H59" s="19"/>
       <c r="I59" s="18"/>
@@ -2545,14 +2545,14 @@
       <c r="K59" s="18"/>
     </row>
     <row r="60" spans="1:11" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="72" t="s">
+      <c r="A60" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
+      <c r="B60" s="73"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
+      <c r="F60" s="73"/>
       <c r="G60" s="1"/>
       <c r="H60" s="19"/>
       <c r="I60" s="18"/>
@@ -2639,7 +2639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="75"/>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -3009,30 +3009,30 @@
       <c r="C29" s="40"/>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="79" t="str">
+      <c r="A30" s="80" t="str">
         <f>Касса!A59</f>
         <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
     </row>
     <row r="31" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80" t="str">
+      <c r="A31" s="81" t="str">
         <f>Касса!A60</f>
         <v>Блюда могут содержать следы молочных продуктов, яичных продуктов, рыбы, моллюсков, кунжута, горчицы, сои, злаков, содержащих глютен, арахиса, аспартама, диоксида серы и сульфатов, люпина, орехов, ракообразных, сельдерея. Допускается использовать аналогичные указанным компоненты, отечественного или импортного производства, соответствующие нормативным и правовым документам Российской Федерации и Таможенного союза.</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
     </row>
     <row r="32" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="74"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
     </row>
     <row r="33" spans="1:3" ht="12.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
     </row>
     <row r="34" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3050,11 +3050,759 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C59"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="88" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41"/>
+      <c r="B1" s="31" t="str">
+        <f>Касса!B2</f>
+        <v>понедельник</v>
+      </c>
+      <c r="C1" s="42"/>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41"/>
+      <c r="B2" s="31" t="str">
+        <f>Касса!B3</f>
+        <v>1 сентября</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <f>Касса!B29</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="45">
+        <f>Касса!A29</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="46">
+        <f>Касса!C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <f>Касса!B30</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="45">
+        <f>Касса!A30</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="46">
+        <f>Касса!C30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <f>Касса!B31</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="45">
+        <f>Касса!A31</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="46">
+        <f>Касса!C31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <f>Касса!B32</f>
+        <v>0</v>
+      </c>
+      <c r="B10" s="45">
+        <f>Касса!A32</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="46">
+        <f>Касса!C32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <f>Касса!B33</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="45">
+        <f>Касса!A33</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="46">
+        <f>Касса!C33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <f>Касса!B34</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="45">
+        <f>Касса!A34</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="46">
+        <f>Касса!C34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <f>Касса!B35</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="45">
+        <f>Касса!A35</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="46">
+        <f>Касса!C35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <f>Касса!B36</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="45">
+        <f>Касса!A36</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="46">
+        <f>Касса!C36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <f>Касса!B37</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="45">
+        <f>Касса!A37</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="46">
+        <f>Касса!C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <f>Касса!B38</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="45">
+        <f>Касса!A38</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="46">
+        <f>Касса!C38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <f>Касса!B39</f>
+        <v>0</v>
+      </c>
+      <c r="B17" s="45">
+        <f>Касса!A39</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="46">
+        <f>Касса!C39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <f>Касса!B40</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="45">
+        <f>Касса!A40</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="46">
+        <f>Касса!C40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <f>Касса!B41</f>
+        <v>0</v>
+      </c>
+      <c r="B19" s="45">
+        <f>Касса!A41</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="46">
+        <f>Касса!C41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="47"/>
+    </row>
+    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <f>Касса!E7</f>
+        <v>0</v>
+      </c>
+      <c r="B21" s="45">
+        <f>Касса!D7</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="46">
+        <f>Касса!F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <f>Касса!E8</f>
+        <v>0</v>
+      </c>
+      <c r="B22" s="45">
+        <f>Касса!D8</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="46">
+        <f>Касса!F8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <f>Касса!E9</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="45">
+        <f>Касса!D9</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="46">
+        <f>Касса!F9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
+        <f>Касса!E10</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="45">
+        <f>Касса!D10</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="46">
+        <f>Касса!F10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="48"/>
+      <c r="B25" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="49"/>
+    </row>
+    <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38">
+        <f>Касса!E12</f>
+        <v>0</v>
+      </c>
+      <c r="B26" s="45">
+        <f>Касса!D12</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="46">
+        <f>Касса!F12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38">
+        <f>Касса!E13</f>
+        <v>0</v>
+      </c>
+      <c r="B27" s="45">
+        <f>Касса!D13</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="46">
+        <f>Касса!F13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="38">
+        <f>Касса!E14</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="45">
+        <f>Касса!D14</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="46">
+        <f>Касса!F14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38">
+        <f>Касса!E15</f>
+        <v>0</v>
+      </c>
+      <c r="B29" s="45">
+        <f>Касса!D15</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="46">
+        <f>Касса!F15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="38">
+        <f>Касса!E16</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="45">
+        <f>Касса!D16</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="46">
+        <f>Касса!F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="38">
+        <f>Касса!E17</f>
+        <v>0</v>
+      </c>
+      <c r="B31" s="45">
+        <f>Касса!D17</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="46">
+        <f>Касса!F17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38"/>
+      <c r="B32" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="50"/>
+    </row>
+    <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <f>Касса!E19</f>
+        <v>0</v>
+      </c>
+      <c r="B33" s="45">
+        <f>Касса!D19</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="46">
+        <f>Касса!F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="38">
+        <f>Касса!E20</f>
+        <v>0</v>
+      </c>
+      <c r="B34" s="45">
+        <f>Касса!D20</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="46">
+        <f>Касса!F20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38">
+        <f>Касса!E21</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="45">
+        <f>Касса!D21</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="46">
+        <f>Касса!F21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="38">
+        <f>Касса!E22</f>
+        <v>0</v>
+      </c>
+      <c r="B36" s="45">
+        <f>Касса!D22</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="46">
+        <f>Касса!F22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="38">
+        <f>Касса!E23</f>
+        <v>0</v>
+      </c>
+      <c r="B37" s="45">
+        <f>Касса!D23</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="46">
+        <f>Касса!F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
+        <f>Касса!E24</f>
+        <v>0</v>
+      </c>
+      <c r="B38" s="45">
+        <f>Касса!D24</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="46">
+        <f>Касса!F24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="38"/>
+      <c r="B39" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="49"/>
+    </row>
+    <row r="40" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="38">
+        <f>Касса!E26</f>
+        <v>0</v>
+      </c>
+      <c r="B40" s="45">
+        <f>Касса!D26</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="46">
+        <f>Касса!F26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="38">
+        <f>Касса!E27</f>
+        <v>0</v>
+      </c>
+      <c r="B41" s="45">
+        <f>Касса!D27</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="46">
+        <f>Касса!F27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38">
+        <f>Касса!E28</f>
+        <v>0</v>
+      </c>
+      <c r="B42" s="45">
+        <f>Касса!D28</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="46">
+        <f>Касса!F28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="38">
+        <f>Касса!E29</f>
+        <v>0</v>
+      </c>
+      <c r="B43" s="45">
+        <f>Касса!D29</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="46">
+        <f>Касса!F29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="51"/>
+      <c r="B44" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="50"/>
+    </row>
+    <row r="45" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="38">
+        <f>Касса!E31</f>
+        <v>0</v>
+      </c>
+      <c r="B45" s="45">
+        <f>Касса!D31</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="46">
+        <f>Касса!F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="38">
+        <f>Касса!E32</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="45">
+        <f>Касса!D32</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="46">
+        <f>Касса!F32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="38">
+        <f>Касса!E33</f>
+        <v>0</v>
+      </c>
+      <c r="B47" s="45">
+        <f>Касса!D33</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="46">
+        <f>Касса!F33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="38">
+        <f>Касса!E34</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="45">
+        <f>Касса!D34</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="46">
+        <f>Касса!F34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
+        <f>Касса!E35</f>
+        <v>0</v>
+      </c>
+      <c r="B49" s="45">
+        <f>Касса!D35</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="46">
+        <f>Касса!F35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="38">
+        <f>Касса!E36</f>
+        <v>0</v>
+      </c>
+      <c r="B50" s="45">
+        <f>Касса!D36</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="46">
+        <f>Касса!F36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="38">
+        <f>Касса!E37</f>
+        <v>0</v>
+      </c>
+      <c r="B51" s="45">
+        <f>Касса!D37</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="46">
+        <f>Касса!F37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="38">
+        <f>Касса!E38</f>
+        <v>0</v>
+      </c>
+      <c r="B52" s="45">
+        <f>Касса!D38</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="46">
+        <f>Касса!F38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="48"/>
+      <c r="B53" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="50"/>
+    </row>
+    <row r="54" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="38" t="str">
+        <f>Касса!E40</f>
+        <v>200/300мл</v>
+      </c>
+      <c r="B54" s="45" t="str">
+        <f>Касса!D40</f>
+        <v>Напиток охл.в стакане/в бутылке</v>
+      </c>
+      <c r="C54" s="46" t="str">
+        <f>Касса!F40</f>
+        <v>60/80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="38" t="str">
+        <f>Касса!E43</f>
+        <v>225мл</v>
+      </c>
+      <c r="B55" s="45" t="str">
+        <f>Касса!D43</f>
+        <v>Чай фруктовый в ассортименте</v>
+      </c>
+      <c r="C55" s="46">
+        <f>Касса!F43</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="80" t="str">
+        <f>Касса!A59</f>
+        <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
+      </c>
+      <c r="B56" s="75"/>
+      <c r="C56" s="75"/>
+    </row>
+    <row r="57" spans="1:3" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="81" t="str">
+        <f>Касса!A60</f>
+        <v>Блюда могут содержать следы молочных продуктов, яичных продуктов, рыбы, моллюсков, кунжута, горчицы, сои, злаков, содержащих глютен, арахиса, аспартама, диоксида серы и сульфатов, люпина, орехов, ракообразных, сельдерея. Допускается использовать аналогичные указанным компоненты, отечественного или импортного производства, соответствующие нормативным и правовым документам Российской Федерации и Таможенного союза.</v>
+      </c>
+      <c r="B57" s="75"/>
+      <c r="C57" s="75"/>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="75"/>
+      <c r="B58" s="75"/>
+      <c r="C58" s="75"/>
+    </row>
+    <row r="59" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="75"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A57:C59"/>
+    <mergeCell ref="A56:C56"/>
+  </mergeCells>
+  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0" bottom="0" header="0.11811023622047249" footer="0.11811023622047249"/>
+  <pageSetup paperSize="9" scale="70" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3082,32 +3830,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="75" t="str">
+      <c r="B2" s="76" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="E2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="str">
+      <c r="B3" s="77" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -3125,15 +3873,15 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -3776,13 +4524,13 @@
       <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="82"/>
-      <c r="B40" s="74"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
       <c r="H40" s="55"/>
       <c r="I40" s="56"/>
       <c r="J40" s="18"/>
@@ -3790,13 +4538,13 @@
       <c r="L40" s="18"/>
     </row>
     <row r="41" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="72"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
       <c r="H41" s="57"/>
       <c r="I41" s="56"/>
       <c r="J41" s="18"/>
@@ -4012,760 +4760,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C59"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.26953125" customWidth="1"/>
-    <col min="2" max="2" width="88" customWidth="1"/>
-    <col min="3" max="3" width="35.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="31" t="str">
-        <f>Касса!B2</f>
-        <v>понедельник</v>
-      </c>
-      <c r="C1" s="42"/>
-    </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="31" t="str">
-        <f>Касса!B3</f>
-        <v>1 сентября</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="69" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="29"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <f>Касса!B29</f>
-        <v>0</v>
-      </c>
-      <c r="B7" s="45">
-        <f>Касса!A29</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="46">
-        <f>Касса!C29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
-        <f>Касса!B30</f>
-        <v>0</v>
-      </c>
-      <c r="B8" s="45">
-        <f>Касса!A30</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="46">
-        <f>Касса!C30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
-        <f>Касса!B31</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="45">
-        <f>Касса!A31</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="46">
-        <f>Касса!C31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <f>Касса!B32</f>
-        <v>0</v>
-      </c>
-      <c r="B10" s="45">
-        <f>Касса!A32</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="46">
-        <f>Касса!C32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
-        <f>Касса!B33</f>
-        <v>0</v>
-      </c>
-      <c r="B11" s="45">
-        <f>Касса!A33</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="46">
-        <f>Касса!C33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
-        <f>Касса!B34</f>
-        <v>0</v>
-      </c>
-      <c r="B12" s="45">
-        <f>Касса!A34</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="46">
-        <f>Касса!C34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
-        <f>Касса!B35</f>
-        <v>0</v>
-      </c>
-      <c r="B13" s="45">
-        <f>Касса!A35</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="46">
-        <f>Касса!C35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
-        <f>Касса!B36</f>
-        <v>0</v>
-      </c>
-      <c r="B14" s="45">
-        <f>Касса!A36</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="46">
-        <f>Касса!C36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
-        <f>Касса!B37</f>
-        <v>0</v>
-      </c>
-      <c r="B15" s="45">
-        <f>Касса!A37</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="46">
-        <f>Касса!C37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
-        <f>Касса!B38</f>
-        <v>0</v>
-      </c>
-      <c r="B16" s="45">
-        <f>Касса!A38</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="46">
-        <f>Касса!C38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
-        <f>Касса!B39</f>
-        <v>0</v>
-      </c>
-      <c r="B17" s="45">
-        <f>Касса!A39</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="46">
-        <f>Касса!C39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
-        <f>Касса!B40</f>
-        <v>0</v>
-      </c>
-      <c r="B18" s="45">
-        <f>Касса!A40</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="46">
-        <f>Касса!C40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
-        <f>Касса!B41</f>
-        <v>0</v>
-      </c>
-      <c r="B19" s="45">
-        <f>Касса!A41</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="46">
-        <f>Касса!C41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="47"/>
-    </row>
-    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
-        <f>Касса!E7</f>
-        <v>0</v>
-      </c>
-      <c r="B21" s="45">
-        <f>Касса!D7</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="46">
-        <f>Касса!F7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
-        <f>Касса!E8</f>
-        <v>0</v>
-      </c>
-      <c r="B22" s="45">
-        <f>Касса!D8</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="46">
-        <f>Касса!F8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
-        <f>Касса!E9</f>
-        <v>0</v>
-      </c>
-      <c r="B23" s="45">
-        <f>Касса!D9</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="46">
-        <f>Касса!F9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
-        <f>Касса!E10</f>
-        <v>0</v>
-      </c>
-      <c r="B24" s="45">
-        <f>Касса!D10</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="46">
-        <f>Касса!F10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="48"/>
-      <c r="B25" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="49"/>
-    </row>
-    <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
-        <f>Касса!E12</f>
-        <v>0</v>
-      </c>
-      <c r="B26" s="45">
-        <f>Касса!D12</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="46">
-        <f>Касса!F12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38">
-        <f>Касса!E13</f>
-        <v>0</v>
-      </c>
-      <c r="B27" s="45">
-        <f>Касса!D13</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="46">
-        <f>Касса!F13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38">
-        <f>Касса!E14</f>
-        <v>0</v>
-      </c>
-      <c r="B28" s="45">
-        <f>Касса!D14</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="46">
-        <f>Касса!F14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38">
-        <f>Касса!E15</f>
-        <v>0</v>
-      </c>
-      <c r="B29" s="45">
-        <f>Касса!D15</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="46">
-        <f>Касса!F15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38">
-        <f>Касса!E16</f>
-        <v>0</v>
-      </c>
-      <c r="B30" s="45">
-        <f>Касса!D16</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="46">
-        <f>Касса!F16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38">
-        <f>Касса!E17</f>
-        <v>0</v>
-      </c>
-      <c r="B31" s="45">
-        <f>Касса!D17</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="46">
-        <f>Касса!F17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="50"/>
-    </row>
-    <row r="33" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38">
-        <f>Касса!E19</f>
-        <v>0</v>
-      </c>
-      <c r="B33" s="45">
-        <f>Касса!D19</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="46">
-        <f>Касса!F19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38">
-        <f>Касса!E20</f>
-        <v>0</v>
-      </c>
-      <c r="B34" s="45">
-        <f>Касса!D20</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="46">
-        <f>Касса!F20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38">
-        <f>Касса!E21</f>
-        <v>0</v>
-      </c>
-      <c r="B35" s="45">
-        <f>Касса!D21</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="46">
-        <f>Касса!F21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38">
-        <f>Касса!E22</f>
-        <v>0</v>
-      </c>
-      <c r="B36" s="45">
-        <f>Касса!D22</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="46">
-        <f>Касса!F22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="38">
-        <f>Касса!E23</f>
-        <v>0</v>
-      </c>
-      <c r="B37" s="45">
-        <f>Касса!D23</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="46">
-        <f>Касса!F23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38">
-        <f>Касса!E24</f>
-        <v>0</v>
-      </c>
-      <c r="B38" s="45">
-        <f>Касса!D24</f>
-        <v>0</v>
-      </c>
-      <c r="C38" s="46">
-        <f>Касса!F24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="49"/>
-    </row>
-    <row r="40" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="38">
-        <f>Касса!E26</f>
-        <v>0</v>
-      </c>
-      <c r="B40" s="45">
-        <f>Касса!D26</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="46">
-        <f>Касса!F26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38">
-        <f>Касса!E27</f>
-        <v>0</v>
-      </c>
-      <c r="B41" s="45">
-        <f>Касса!D27</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="46">
-        <f>Касса!F27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38">
-        <f>Касса!E28</f>
-        <v>0</v>
-      </c>
-      <c r="B42" s="45">
-        <f>Касса!D28</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="46">
-        <f>Касса!F28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38">
-        <f>Касса!E29</f>
-        <v>0</v>
-      </c>
-      <c r="B43" s="45">
-        <f>Касса!D29</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="46">
-        <f>Касса!F29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="51"/>
-      <c r="B44" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="50"/>
-    </row>
-    <row r="45" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38">
-        <f>Касса!E31</f>
-        <v>0</v>
-      </c>
-      <c r="B45" s="45">
-        <f>Касса!D31</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="46">
-        <f>Касса!F31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38">
-        <f>Касса!E32</f>
-        <v>0</v>
-      </c>
-      <c r="B46" s="45">
-        <f>Касса!D32</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="46">
-        <f>Касса!F32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="38">
-        <f>Касса!E33</f>
-        <v>0</v>
-      </c>
-      <c r="B47" s="45">
-        <f>Касса!D33</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="46">
-        <f>Касса!F33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38">
-        <f>Касса!E34</f>
-        <v>0</v>
-      </c>
-      <c r="B48" s="45">
-        <f>Касса!D34</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="46">
-        <f>Касса!F34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="38">
-        <f>Касса!E35</f>
-        <v>0</v>
-      </c>
-      <c r="B49" s="45">
-        <f>Касса!D35</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="46">
-        <f>Касса!F35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="38">
-        <f>Касса!E36</f>
-        <v>0</v>
-      </c>
-      <c r="B50" s="45">
-        <f>Касса!D36</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="46">
-        <f>Касса!F36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="38">
-        <f>Касса!E37</f>
-        <v>0</v>
-      </c>
-      <c r="B51" s="45">
-        <f>Касса!D37</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="46">
-        <f>Касса!F37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="38">
-        <f>Касса!E38</f>
-        <v>0</v>
-      </c>
-      <c r="B52" s="45">
-        <f>Касса!D38</f>
-        <v>0</v>
-      </c>
-      <c r="C52" s="46">
-        <f>Касса!F38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="48"/>
-      <c r="B53" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="50"/>
-    </row>
-    <row r="54" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="str">
-        <f>Касса!E40</f>
-        <v>200/300мл</v>
-      </c>
-      <c r="B54" s="45" t="str">
-        <f>Касса!D40</f>
-        <v>Напиток охл.в стакане/в бутылке</v>
-      </c>
-      <c r="C54" s="46" t="str">
-        <f>Касса!F40</f>
-        <v>60/80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="str">
-        <f>Касса!E43</f>
-        <v>225мл</v>
-      </c>
-      <c r="B55" s="45" t="str">
-        <f>Касса!D43</f>
-        <v>Чай фруктовый в ассортименте</v>
-      </c>
-      <c r="C55" s="46">
-        <f>Касса!F43</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="79" t="str">
-        <f>Касса!A59</f>
-        <v>*ПРИ НАЛИЧИИ У ВАС АЛЛЕРГИИ, УТОЧНЯЙТЕ ИНФОРМАЦИЮ О ПОДРОБНОМ СОСТАВЕ БЛЮД В МЕНЮ С ВЫХОДОМ НА ДОСКЕ ПОТРЕБИТЕЛЯ.</v>
-      </c>
-      <c r="B56" s="74"/>
-      <c r="C56" s="74"/>
-    </row>
-    <row r="57" spans="1:3" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="80" t="str">
-        <f>Касса!A60</f>
-        <v>Блюда могут содержать следы молочных продуктов, яичных продуктов, рыбы, моллюсков, кунжута, горчицы, сои, злаков, содержащих глютен, арахиса, аспартама, диоксида серы и сульфатов, люпина, орехов, ракообразных, сельдерея. Допускается использовать аналогичные указанным компоненты, отечественного или импортного производства, соответствующие нормативным и правовым документам Российской Федерации и Таможенного союза.</v>
-      </c>
-      <c r="B57" s="74"/>
-      <c r="C57" s="74"/>
-    </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="74"/>
-      <c r="B58" s="74"/>
-      <c r="C58" s="74"/>
-    </row>
-    <row r="59" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="74"/>
-      <c r="B59" s="74"/>
-      <c r="C59" s="74"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A57:C59"/>
-    <mergeCell ref="A56:C56"/>
-  </mergeCells>
-  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0" bottom="0" header="0.11811023622047249" footer="0.11811023622047249"/>
-  <pageSetup paperSize="9" scale="70" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4793,32 +4793,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="75" t="str">
+      <c r="B2" s="76" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="E2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="str">
+      <c r="B3" s="77" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -4836,15 +4836,15 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -4872,12 +4872,12 @@
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="str">
-        <f>Касса!A28</f>
-        <v>САЛАТЫ и ХОЛОДНЫЕ ЗАКУСКИ</v>
+      <c r="A7" s="6">
+        <f>Касса!A29</f>
+        <v>0</v>
       </c>
       <c r="B7" s="3">
-        <f>Касса!B28</f>
+        <f>Касса!B29</f>
         <v>0</v>
       </c>
       <c r="C7" s="15"/>
@@ -4893,11 +4893,11 @@
     </row>
     <row r="8" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <f>Касса!A29</f>
+        <f>Касса!A30</f>
         <v>0</v>
       </c>
       <c r="B8" s="3">
-        <f>Касса!B29</f>
+        <f>Касса!B30</f>
         <v>0</v>
       </c>
       <c r="C8" s="15"/>
@@ -4913,11 +4913,11 @@
     </row>
     <row r="9" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
-        <f>Касса!A30</f>
+        <f>Касса!A31</f>
         <v>0</v>
       </c>
       <c r="B9" s="3">
-        <f>Касса!B30</f>
+        <f>Касса!B31</f>
         <v>0</v>
       </c>
       <c r="C9" s="15"/>
@@ -4933,11 +4933,11 @@
     </row>
     <row r="10" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <f>Касса!A31</f>
+        <f>Касса!A32</f>
         <v>0</v>
       </c>
       <c r="B10" s="3">
-        <f>Касса!B31</f>
+        <f>Касса!B32</f>
         <v>0</v>
       </c>
       <c r="C10" s="15"/>
@@ -4953,11 +4953,11 @@
     </row>
     <row r="11" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
-        <f>Касса!A32</f>
+        <f>Касса!A33</f>
         <v>0</v>
       </c>
       <c r="B11" s="3">
-        <f>Касса!B32</f>
+        <f>Касса!B33</f>
         <v>0</v>
       </c>
       <c r="C11" s="15"/>
@@ -4973,11 +4973,11 @@
     </row>
     <row r="12" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <f>Касса!A33</f>
+        <f>Касса!A34</f>
         <v>0</v>
       </c>
       <c r="B12" s="3">
-        <f>Касса!B33</f>
+        <f>Касса!B34</f>
         <v>0</v>
       </c>
       <c r="C12" s="15"/>
@@ -4993,11 +4993,11 @@
     </row>
     <row r="13" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
-        <f>Касса!A34</f>
+        <f>Касса!A35</f>
         <v>0</v>
       </c>
       <c r="B13" s="3">
-        <f>Касса!B34</f>
+        <f>Касса!B35</f>
         <v>0</v>
       </c>
       <c r="C13" s="15"/>
@@ -5013,11 +5013,11 @@
     </row>
     <row r="14" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <f>Касса!A35</f>
+        <f>Касса!A36</f>
         <v>0</v>
       </c>
       <c r="B14" s="3">
-        <f>Касса!B35</f>
+        <f>Касса!B36</f>
         <v>0</v>
       </c>
       <c r="C14" s="15"/>
@@ -5033,11 +5033,11 @@
     </row>
     <row r="15" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
-        <f>Касса!A36</f>
+        <f>Касса!A37</f>
         <v>0</v>
       </c>
       <c r="B15" s="3">
-        <f>Касса!B36</f>
+        <f>Касса!B37</f>
         <v>0</v>
       </c>
       <c r="C15" s="15"/>
@@ -5053,11 +5053,11 @@
     </row>
     <row r="16" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
-        <f>Касса!A37</f>
+        <f>Касса!A38</f>
         <v>0</v>
       </c>
       <c r="B16" s="3">
-        <f>Касса!B37</f>
+        <f>Касса!B38</f>
         <v>0</v>
       </c>
       <c r="C16" s="61"/>
@@ -5073,11 +5073,11 @@
     </row>
     <row r="17" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <f>Касса!A38</f>
+        <f>Касса!A39</f>
         <v>0</v>
       </c>
       <c r="B17" s="3">
-        <f>Касса!B38</f>
+        <f>Касса!B39</f>
         <v>0</v>
       </c>
       <c r="C17" s="15"/>
@@ -5093,11 +5093,11 @@
     </row>
     <row r="18" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <f>Касса!A39</f>
+        <f>Касса!A40</f>
         <v>0</v>
       </c>
       <c r="B18" s="3">
-        <f>Касса!B39</f>
+        <f>Касса!B40</f>
         <v>0</v>
       </c>
       <c r="C18" s="61"/>
@@ -5113,14 +5113,16 @@
     </row>
     <row r="19" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
-        <f>Касса!A40</f>
+        <f>Касса!A41</f>
         <v>0</v>
       </c>
       <c r="B19" s="3">
-        <f>Касса!B40</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="15"/>
+        <f>Касса!B41</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>77</v>
+      </c>
       <c r="D19" s="62"/>
       <c r="E19" s="10"/>
       <c r="F19" s="15"/>
@@ -5132,16 +5134,18 @@
       <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
-        <f>Касса!A41</f>
-        <v>0</v>
-      </c>
-      <c r="B20" s="3">
-        <f>Касса!B41</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="A20" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53">
+        <f>SUM(C7:D19)+4+4</f>
+        <v>8</v>
+      </c>
+      <c r="D20" s="53">
+        <f ca="1">SUM(D7:E20)+4+4</f>
+        <v>0</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
@@ -5152,14 +5156,10 @@
       <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53">
-        <f>SUM(C7:D20)+4+4</f>
-        <v>8</v>
-      </c>
+      <c r="A21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="15"/>
       <c r="D21" s="53"/>
       <c r="E21" s="10"/>
       <c r="F21" s="15"/>
@@ -5171,11 +5171,17 @@
       <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="A22" s="6" t="str">
+        <f>Касса!A43</f>
+        <v>Сэндвич с бужениной</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>Касса!B43</f>
+        <v>180г</v>
+      </c>
+      <c r="C22" s="15">
+        <v>2</v>
+      </c>
       <c r="D22" s="53"/>
       <c r="E22" s="10"/>
       <c r="F22" s="15"/>
@@ -5188,15 +5194,15 @@
     </row>
     <row r="23" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="str">
-        <f>Касса!A43</f>
-        <v>Сэндвич с бужениной</v>
+        <f>Касса!A44</f>
+        <v>Сэндвич с ветчиной и сыром</v>
       </c>
       <c r="B23" s="3" t="str">
-        <f>Касса!B43</f>
+        <f>Касса!B44</f>
         <v>180г</v>
       </c>
       <c r="C23" s="15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="10"/>
@@ -5210,11 +5216,11 @@
     </row>
     <row r="24" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="str">
-        <f>Касса!A44</f>
-        <v>Сэндвич с ветчиной и сыром</v>
+        <f>Касса!A45</f>
+        <v>Сэндвич с куриной грудкой</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f>Касса!B44</f>
+        <f>Касса!B45</f>
         <v>180г</v>
       </c>
       <c r="C24" s="15">
@@ -5232,15 +5238,15 @@
     </row>
     <row r="25" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="str">
-        <f>Касса!A45</f>
-        <v>Сэндвич с куриной грудкой</v>
+        <f>Касса!A46</f>
+        <v>Сэндвич с форелью</v>
       </c>
       <c r="B25" s="3" t="str">
-        <f>Касса!B45</f>
+        <f>Касса!B46</f>
         <v>180г</v>
       </c>
       <c r="C25" s="15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D25" s="53"/>
       <c r="E25" s="53"/>
@@ -5253,21 +5259,10 @@
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="str">
-        <f>Касса!A46</f>
-        <v>Сэндвич с форелью</v>
-      </c>
-      <c r="B26" s="3" t="str">
-        <f>Касса!B46</f>
-        <v>180г</v>
-      </c>
-      <c r="C26" s="15">
-        <v>2</v>
-      </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="84"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
       <c r="H26" s="19"/>
       <c r="I26" s="20"/>
       <c r="J26" s="18"/>
@@ -5275,10 +5270,7 @@
       <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
+      <c r="A27" s="28"/>
       <c r="H27" s="19"/>
       <c r="I27" s="20"/>
       <c r="J27" s="18"/>
@@ -5287,14 +5279,12 @@
     </row>
     <row r="28" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
       <c r="H28" s="20"/>
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
       <c r="H29" s="19"/>
       <c r="I29" s="20"/>
       <c r="J29" s="18"/>
@@ -5302,7 +5292,6 @@
       <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
       <c r="H30" s="19"/>
       <c r="I30" s="20"/>
       <c r="J30" s="18"/>
@@ -5575,8 +5564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5604,32 +5593,32 @@
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="75" t="str">
+      <c r="B2" s="76" t="str">
         <f>Касса!B2</f>
         <v>понедельник</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="E2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="str">
+      <c r="B3" s="77" t="str">
         <f>Касса!B3</f>
         <v>1 сентября</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -5647,15 +5636,15 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="1"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -6362,12 +6351,12 @@
         <f>Касса!A41</f>
         <v>0</v>
       </c>
-      <c r="B41" s="83"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
       <c r="H41" s="57"/>
       <c r="I41" s="56"/>
       <c r="J41" s="63"/>

</xml_diff>